<commit_message>
feat: 完成 2026-01-16 每日定投分析 (Gemini-Pro)
</commit_message>
<xml_diff>
--- a/Data/投资策略.xlsx
+++ b/Data/投资策略.xlsx
@@ -8,12 +8,12 @@
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr fullCalcOnLoad="true"/>
+  <calcPr fullCalcOnLoad="false"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="104">
   <si>
     <t/>
   </si>
@@ -120,6 +120,9 @@
     <t>消费电子</t>
   </si>
   <si>
+    <t>015876</t>
+  </si>
+  <si>
     <t>富国中证消费电子主题ETF联接A</t>
   </si>
   <si>
@@ -211,6 +214,21 @@
   </si>
   <si>
     <t>广发港股创新药ETF联接(QDII)A</t>
+  </si>
+  <si>
+    <t>红利低波</t>
+  </si>
+  <si>
+    <t>007466</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 华泰柏瑞中证红利低波动ETF联接A</t>
+  </si>
+  <si>
+    <t>长期稳定</t>
+  </si>
+  <si>
+    <t>银行估值稍高有下行风险</t>
   </si>
   <si>
     <t>有色</t>
@@ -335,7 +353,7 @@
       <name val="Microsoft YaHei"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -407,6 +425,22 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFF9E3"/>
+        <bgColor auto="true"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEAFAF1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF9E3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFDCC4"/>
       </patternFill>
     </fill>
@@ -429,7 +463,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -481,6 +515,9 @@
     <xf fontId="0" fillId="4" borderId="1" xfId="0">
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="false" shrinkToFit="false"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="false" shrinkToFit="false"/>
     </xf>
@@ -538,16 +575,25 @@
     <xf fontId="0" fillId="13" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
+    <xf fontId="0" fillId="14" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="false" shrinkToFit="false"/>
+    </xf>
+    <xf fontId="0" fillId="15" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf fontId="0" fillId="16" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
     <xf fontId="0" fillId="4" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="false" shrinkToFit="false"/>
     </xf>
     <xf fontId="0" fillId="12" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" justifyLastLine="false" shrinkToFit="false"/>
     </xf>
-    <xf fontId="0" fillId="14" borderId="0" xfId="0">
+    <xf fontId="0" fillId="17" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="15" borderId="0" xfId="0">
+    <xf fontId="0" fillId="18" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="false" shrinkToFit="false"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" xfId="0">
@@ -799,7 +845,7 @@
   <sheetPr>
     <tabColor/>
   </sheetPr>
-  <dimension ref="L207"/>
+  <dimension ref="L208"/>
   <sheetViews>
     <sheetView showGridLines="true" rightToLeft="false" workbookViewId="0"/>
   </sheetViews>
@@ -810,7 +856,7 @@
     <col min="3" max="3" width="13.7109" customWidth="true"/>
     <col min="4" max="4" width="15.5938" customWidth="true"/>
     <col min="5" max="5" width="8.40234" customWidth="true"/>
-    <col min="6" max="6" width="28.7109" customWidth="true"/>
+    <col min="6" max="6" width="29.4219" customWidth="true"/>
     <col min="7" max="7" width="12.8125" customWidth="true"/>
     <col min="8" max="8" width="13.7109" customWidth="true"/>
     <col min="9" max="9" width="28.7109" customWidth="true"/>
@@ -1006,31 +1052,32 @@
       <c r="D10" s="11">
         <v>0.5</v>
       </c>
-      <c r="E10" s="7" t="s"/>
-      <c r="F10" s="17" t="s">
+      <c r="E10" s="17" t="s"/>
+      <c r="F10" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="17">
+      <c r="G10" s="18">
         <f>=E3*C3*D10</f>
-      </c>
-      <c r="H10" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="H10" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="I10" s="19" t="s">
+      <c r="I10" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="J10" s="20" t="s">
+      <c r="J10" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="K10" s="21" t="s">
+      <c r="K10" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="L10" s="17">
+      <c r="L10" s="18">
         <v>2305.55</v>
       </c>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="22" t="s"/>
+      <c r="A11" s="23" t="s"/>
       <c r="B11" s="15" t="s">
         <v>5</v>
       </c>
@@ -1040,26 +1087,27 @@
       <c r="D11" s="11">
         <v>0.5</v>
       </c>
-      <c r="E11" s="7" t="s"/>
-      <c r="F11" s="17" t="s">
+      <c r="E11" s="17" t="s"/>
+      <c r="F11" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="G11" s="17">
+      <c r="G11" s="18">
         <f>=E3*C3*D11</f>
-      </c>
-      <c r="H11" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="H11" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="I11" s="19" t="s">
+      <c r="I11" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="J11" s="20" t="s">
+      <c r="J11" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="K11" s="21" t="s">
+      <c r="K11" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="L11" s="17">
+      <c r="L11" s="18">
         <v>1961.24</v>
       </c>
     </row>
@@ -1068,47 +1116,48 @@
       <c r="B12" s="4" t="s"/>
       <c r="C12" s="4" t="s"/>
       <c r="D12" s="4" t="s"/>
-      <c r="E12" s="7" t="s"/>
+      <c r="E12" s="17" t="s"/>
       <c r="F12" s="7" t="s"/>
       <c r="G12" s="7" t="s"/>
       <c r="H12" s="4" t="s"/>
-      <c r="I12" s="24" t="s"/>
-      <c r="J12" s="24" t="s"/>
-      <c r="K12" s="24" t="s"/>
+      <c r="I12" s="25" t="s"/>
+      <c r="J12" s="25" t="s"/>
+      <c r="K12" s="25" t="s"/>
       <c r="L12" s="7" t="s"/>
     </row>
     <row r="13" spans="2:12">
       <c r="B13" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="26" t="s">
         <v>27</v>
       </c>
       <c r="D13" s="11">
-        <v>0.15</v>
-      </c>
-      <c r="E13" s="26" t="s">
+        <v>0.12</v>
+      </c>
+      <c r="E13" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="F13" s="17" t="s">
+      <c r="F13" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="G13" s="17">
+      <c r="G13" s="18">
         <f>=E3*C4*D13</f>
-      </c>
-      <c r="H13" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="H13" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="I13" s="20" t="s">
+      <c r="I13" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="J13" s="20" t="s">
+      <c r="J13" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="K13" s="20" t="s">
+      <c r="K13" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="L13" s="17">
+      <c r="L13" s="18">
         <v>1365.83</v>
       </c>
     </row>
@@ -1116,653 +1165,689 @@
       <c r="B14" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="25" t="s">
+      <c r="C14" s="26" t="s">
         <v>34</v>
       </c>
       <c r="D14" s="11">
-        <v>0.15</v>
-      </c>
-      <c r="E14" s="7" t="s"/>
-      <c r="F14" s="17" t="s">
+        <v>0.13</v>
+      </c>
+      <c r="E14" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="G14" s="17">
+      <c r="F14" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14" s="18">
         <f>=E3*C4*D14</f>
-      </c>
-      <c r="H14" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="I14" s="20" t="s">
+        <v>45.5</v>
+      </c>
+      <c r="H14" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="J14" s="20" t="s">
+      <c r="I14" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="K14" s="20" t="s">
+      <c r="J14" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="L14" s="17">
+      <c r="K14" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="L14" s="18">
         <v>1853.09</v>
       </c>
     </row>
     <row r="15" spans="2:12">
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="30" t="s">
-        <v>40</v>
+      <c r="C15" s="31" t="s">
+        <v>41</v>
       </c>
       <c r="D15" s="11">
         <v>0.2</v>
       </c>
-      <c r="E15" s="7" t="s"/>
-      <c r="F15" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="G15" s="31">
+      <c r="E15" s="17" t="s"/>
+      <c r="F15" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" s="32">
         <f>=E3*C4*D15</f>
-      </c>
-      <c r="H15" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="H15" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="I15" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="J15" s="19" t="s">
+      <c r="I15" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="K15" s="20" t="s">
+      <c r="J15" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="L15" s="17">
+      <c r="K15" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="L15" s="18">
         <v>4227.59</v>
       </c>
     </row>
     <row r="16" spans="2:12">
-      <c r="B16" s="29" t="s">
+      <c r="B16" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="32" t="s">
-        <v>45</v>
+      <c r="C16" s="33" t="s">
+        <v>46</v>
       </c>
       <c r="D16" s="11">
-        <v>0.15</v>
-      </c>
-      <c r="E16" s="7" t="s"/>
-      <c r="F16" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="G16" s="17">
+        <v>0.1</v>
+      </c>
+      <c r="E16" s="17" t="s"/>
+      <c r="F16" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" s="18">
         <f>=E3*C4*D16</f>
-      </c>
-      <c r="H16" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="H16" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="I16" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="J16" s="20" t="s">
+      <c r="I16" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="K16" s="19" t="s">
+      <c r="J16" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="L16" s="17">
+      <c r="K16" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="L16" s="18">
         <v>2004.37</v>
       </c>
     </row>
     <row r="17" spans="2:12">
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="32" t="s">
-        <v>50</v>
+      <c r="C17" s="33" t="s">
+        <v>51</v>
       </c>
       <c r="D17" s="11">
         <v>0.15</v>
       </c>
-      <c r="E17" s="7" t="s"/>
-      <c r="F17" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="G17" s="17">
+      <c r="E17" s="17" t="s"/>
+      <c r="F17" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="G17" s="18">
         <f>=E3*C4*D17</f>
-      </c>
-      <c r="H17" s="23" t="s">
+        <v>52.5</v>
+      </c>
+      <c r="H17" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="I17" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="J17" s="20" t="s">
+      <c r="I17" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="K17" s="19" t="s">
+      <c r="J17" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="L17" s="17">
+      <c r="K17" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="L17" s="18">
         <v>1454.78</v>
       </c>
     </row>
     <row r="18" spans="2:12" ht="25.5" customHeight="true">
-      <c r="B18" s="29" t="s">
+      <c r="B18" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="30" t="s">
-        <v>55</v>
+      <c r="C18" s="31" t="s">
+        <v>56</v>
       </c>
       <c r="D18" s="11">
         <v>0.1</v>
       </c>
-      <c r="E18" s="7" t="s"/>
-      <c r="F18" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="G18" s="17">
+      <c r="E18" s="17" t="s"/>
+      <c r="F18" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="G18" s="18">
         <f>=E3*C4*D18</f>
-      </c>
-      <c r="H18" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="H18" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="I18" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="J18" s="20" t="s">
+      <c r="I18" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="K18" s="19" t="s">
+      <c r="J18" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="L18" s="17">
+      <c r="K18" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="L18" s="18">
         <v>41.4</v>
       </c>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" s="4" t="s"/>
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="D19" s="33">
+      <c r="C19" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="34">
         <v>0.05</v>
       </c>
-      <c r="E19" s="7" t="s"/>
-      <c r="F19" s="17" t="s">
-        <v>61</v>
+      <c r="E19" s="17" t="s"/>
+      <c r="F19" s="18" t="s">
+        <v>62</v>
       </c>
       <c r="G19" s="7">
         <f>=E3*C4*D19</f>
-      </c>
-      <c r="H19" s="18" t="s">
+        <v>17.5</v>
+      </c>
+      <c r="H19" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="I19" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="J19" s="34" t="s">
+      <c r="I19" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="K19" s="35" t="s">
+      <c r="J19" s="35" t="s">
         <v>64</v>
+      </c>
+      <c r="K19" s="36" t="s">
+        <v>65</v>
       </c>
       <c r="L19" s="7" t="s"/>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" s="4" t="s"/>
-      <c r="B20" s="29" t="s">
+      <c r="B20" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="D20" s="33">
+      <c r="C20" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="34">
         <v>0.05</v>
       </c>
-      <c r="E20" s="7" t="s"/>
-      <c r="F20" s="17" t="s">
-        <v>65</v>
+      <c r="E20" s="17" t="s"/>
+      <c r="F20" s="18" t="s">
+        <v>66</v>
       </c>
       <c r="G20" s="7">
         <f>=E3*C4*D20</f>
-      </c>
-      <c r="H20" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="I20" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="J20" s="34" t="s">
+        <v>17.5</v>
+      </c>
+      <c r="H20" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="I20" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="K20" s="35" t="s">
+      <c r="J20" s="35" t="s">
         <v>64</v>
+      </c>
+      <c r="K20" s="36" t="s">
+        <v>65</v>
       </c>
       <c r="L20" s="7" t="s"/>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="4" t="s"/>
-      <c r="B21" s="7" t="s"/>
-      <c r="C21" s="4" t="s"/>
-      <c r="D21" s="4" t="s"/>
-      <c r="E21" s="7" t="s"/>
-      <c r="F21" s="7" t="s"/>
-      <c r="G21" s="7" t="s"/>
-      <c r="H21" s="4" t="s"/>
-      <c r="I21" s="24" t="s"/>
-      <c r="J21" s="24" t="s"/>
-      <c r="K21" s="24" t="s"/>
+      <c r="B21" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="34">
+        <v>0.1</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="G21" s="7">
+        <f>=E3*C4*D21</f>
+        <v>35</v>
+      </c>
+      <c r="H21" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I21" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="J21" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="K21" s="35" t="s">
+        <v>64</v>
+      </c>
       <c r="L21" s="7" t="s"/>
     </row>
     <row r="22" spans="1:12">
-      <c r="A22" s="15" t="s"/>
-      <c r="B22" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" s="36" t="s">
-        <v>66</v>
-      </c>
-      <c r="D22" s="11">
-        <v>0.3</v>
-      </c>
-      <c r="E22" s="7" t="s"/>
-      <c r="F22" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="G22" s="31">
-        <f>=E3*C4*D13</f>
-      </c>
-      <c r="H22" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="I22" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="J22" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="K22" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="L22" s="17">
-        <v>2780.07</v>
-      </c>
+      <c r="A22" s="4" t="s"/>
+      <c r="B22" s="7" t="s"/>
+      <c r="C22" s="4" t="s"/>
+      <c r="D22" s="4" t="s"/>
+      <c r="E22" s="17" t="s"/>
+      <c r="F22" s="7" t="s"/>
+      <c r="G22" s="7" t="s"/>
+      <c r="H22" s="4" t="s"/>
+      <c r="I22" s="25" t="s"/>
+      <c r="J22" s="25" t="s"/>
+      <c r="K22" s="25" t="s"/>
+      <c r="L22" s="7" t="s"/>
     </row>
     <row r="23" spans="1:12">
-      <c r="A23" s="22" t="s"/>
+      <c r="A23" s="15" t="s"/>
       <c r="B23" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="36" t="s">
-        <v>70</v>
+      <c r="C23" s="40" t="s">
+        <v>72</v>
       </c>
       <c r="D23" s="11">
-        <v>0.1</v>
-      </c>
-      <c r="E23" s="7" t="s"/>
-      <c r="F23" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="G23" s="17">
+        <v>0.3</v>
+      </c>
+      <c r="E23" s="17" t="s"/>
+      <c r="F23" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="G23" s="32">
         <f>=E3*C5*D23</f>
-      </c>
-      <c r="H23" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="I23" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="J23" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="K23" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="L23" s="17">
-        <v>1897.31</v>
+        <v>60</v>
+      </c>
+      <c r="H23" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="I23" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="J23" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="K23" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="L23" s="18">
+        <v>2780.07</v>
       </c>
     </row>
     <row r="24" spans="1:12">
-      <c r="A24" s="22" t="s"/>
+      <c r="A24" s="23" t="s"/>
       <c r="B24" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="36" t="s">
-        <v>73</v>
+      <c r="C24" s="40" t="s">
+        <v>76</v>
       </c>
       <c r="D24" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="E24" s="17" t="s"/>
+      <c r="F24" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="G24" s="18">
+        <f>=E3*C5*D24</f>
+        <v>20</v>
+      </c>
+      <c r="H24" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="I24" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="J24" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="K24" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="L24" s="18">
+        <v>1897.31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="23" t="s"/>
+      <c r="B25" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="40" t="s">
+        <v>79</v>
+      </c>
+      <c r="D25" s="11">
         <v>0.6</v>
       </c>
-      <c r="E24" s="7" t="s"/>
-      <c r="F24" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="G24" s="17">
-        <f>=E3*C5*D24</f>
-      </c>
-      <c r="H24" s="27" t="s">
+      <c r="E25" s="17" t="s"/>
+      <c r="F25" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="G25" s="18">
+        <f>=E3*C5*D25</f>
+        <v>120</v>
+      </c>
+      <c r="H25" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="I24" s="20" t="s">
+      <c r="I25" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="J25" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="J24" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="K24" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="L24" s="17">
+      <c r="K25" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="L25" s="18">
         <v>4046.83</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
-      <c r="A25" s="4" t="s"/>
-      <c r="B25" s="4" t="s"/>
-      <c r="C25" s="4" t="s"/>
-      <c r="D25" s="4" t="s"/>
-      <c r="E25" s="7" t="s"/>
-      <c r="F25" s="7" t="s"/>
-      <c r="G25" s="7" t="s"/>
-      <c r="H25" s="4" t="s"/>
-      <c r="I25" s="24" t="s"/>
-      <c r="J25" s="24" t="s"/>
-      <c r="K25" s="24" t="s"/>
-      <c r="L25" s="7" t="s"/>
-    </row>
     <row r="26" spans="1:12">
-      <c r="A26" s="15" t="s"/>
-      <c r="B26" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C26" s="36" t="s">
-        <v>76</v>
-      </c>
-      <c r="D26" s="11">
-        <v>0.33</v>
-      </c>
-      <c r="E26" s="7" t="s"/>
-      <c r="F26" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="G26" s="17">
-        <f>=E3*C6*D26</f>
-      </c>
-      <c r="H26" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="I26" s="37" t="s">
-        <v>78</v>
-      </c>
-      <c r="J26" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="K26" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="L26" s="17">
-        <v>1754.33</v>
-      </c>
+      <c r="A26" s="4" t="s"/>
+      <c r="B26" s="4" t="s"/>
+      <c r="C26" s="4" t="s"/>
+      <c r="D26" s="4" t="s"/>
+      <c r="E26" s="17" t="s"/>
+      <c r="F26" s="7" t="s"/>
+      <c r="G26" s="7" t="s"/>
+      <c r="H26" s="4" t="s"/>
+      <c r="I26" s="25" t="s"/>
+      <c r="J26" s="25" t="s"/>
+      <c r="K26" s="25" t="s"/>
+      <c r="L26" s="7" t="s"/>
     </row>
     <row r="27" spans="1:12">
-      <c r="A27" s="22" t="s"/>
+      <c r="A27" s="15" t="s"/>
       <c r="B27" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="36" t="s">
-        <v>76</v>
+      <c r="C27" s="40" t="s">
+        <v>82</v>
       </c>
       <c r="D27" s="11">
         <v>0.33</v>
       </c>
-      <c r="E27" s="7" t="s"/>
-      <c r="F27" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="G27" s="17">
+      <c r="E27" s="17" t="s"/>
+      <c r="F27" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="G27" s="18">
         <f>=E3*C6*D27</f>
-      </c>
-      <c r="H27" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="I27" s="37" t="s">
-        <v>78</v>
-      </c>
-      <c r="J27" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="K27" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="L27" s="17">
-        <v>1402.87</v>
+        <v>66</v>
+      </c>
+      <c r="H27" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="I27" s="41" t="s">
+        <v>84</v>
+      </c>
+      <c r="J27" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="K27" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="L27" s="18">
+        <v>1754.33</v>
       </c>
     </row>
     <row r="28" spans="1:12">
-      <c r="A28" s="22" t="s"/>
+      <c r="A28" s="23" t="s"/>
       <c r="B28" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C28" s="32" t="s">
+      <c r="C28" s="40" t="s">
         <v>82</v>
       </c>
       <c r="D28" s="11">
         <v>0.33</v>
       </c>
-      <c r="E28" s="7" t="s"/>
-      <c r="F28" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="G28" s="17">
+      <c r="E28" s="17" t="s"/>
+      <c r="F28" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="G28" s="18">
         <f>=E3*C6*D28</f>
-      </c>
-      <c r="H28" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="I28" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="H28" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I28" s="41" t="s">
         <v>84</v>
       </c>
-      <c r="J28" s="21" t="s">
+      <c r="J28" s="22" t="s">
         <v>85</v>
       </c>
       <c r="K28" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="L28" s="17">
+      <c r="L28" s="18">
+        <v>1402.87</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="23" t="s"/>
+      <c r="B29" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29" s="11">
+        <v>0.33</v>
+      </c>
+      <c r="E29" s="17" t="s"/>
+      <c r="F29" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="G29" s="18">
+        <f>=E3*C6*D29</f>
+        <v>66</v>
+      </c>
+      <c r="H29" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="I29" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="J29" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="K29" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="L29" s="18">
         <v>2521.47</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
-      <c r="A29" s="7" t="s"/>
-      <c r="B29" s="7" t="s"/>
-      <c r="C29" s="4" t="s"/>
-      <c r="D29" s="4" t="s"/>
-      <c r="E29" s="7" t="s"/>
-      <c r="F29" s="7" t="s"/>
-      <c r="G29" s="7" t="s"/>
-      <c r="H29" s="4" t="s"/>
-      <c r="I29" s="24" t="s"/>
-      <c r="J29" s="24" t="s"/>
-      <c r="K29" s="24" t="s"/>
-      <c r="L29" s="7" t="s"/>
-    </row>
     <row r="30" spans="1:12">
-      <c r="A30" s="4" t="s"/>
-      <c r="B30" s="4" t="s"/>
+      <c r="A30" s="7" t="s"/>
+      <c r="B30" s="7" t="s"/>
       <c r="C30" s="4" t="s"/>
       <c r="D30" s="4" t="s"/>
       <c r="E30" s="7" t="s"/>
       <c r="F30" s="7" t="s"/>
       <c r="G30" s="7" t="s"/>
       <c r="H30" s="4" t="s"/>
-      <c r="I30" s="24" t="s"/>
-      <c r="J30" s="24" t="s"/>
-      <c r="K30" s="24" t="s"/>
+      <c r="I30" s="25" t="s"/>
+      <c r="J30" s="25" t="s"/>
+      <c r="K30" s="25" t="s"/>
       <c r="L30" s="7" t="s"/>
     </row>
     <row r="31" spans="1:12">
       <c r="A31" s="4" t="s"/>
-      <c r="B31" s="38" t="s">
-        <v>87</v>
-      </c>
+      <c r="B31" s="4" t="s"/>
       <c r="C31" s="4" t="s"/>
       <c r="D31" s="4" t="s"/>
       <c r="E31" s="7" t="s"/>
       <c r="F31" s="7" t="s"/>
       <c r="G31" s="7" t="s"/>
       <c r="H31" s="4" t="s"/>
-      <c r="I31" s="24" t="s"/>
-      <c r="J31" s="24" t="s"/>
-      <c r="K31" s="24" t="s"/>
+      <c r="I31" s="25" t="s"/>
+      <c r="J31" s="25" t="s"/>
+      <c r="K31" s="25" t="s"/>
       <c r="L31" s="7" t="s"/>
     </row>
     <row r="32" spans="1:12">
       <c r="A32" s="4" t="s"/>
-      <c r="B32" s="12" t="s">
+      <c r="B32" s="42" t="s">
+        <v>93</v>
+      </c>
+      <c r="C32" s="4" t="s"/>
+      <c r="D32" s="4" t="s"/>
+      <c r="E32" s="7" t="s"/>
+      <c r="F32" s="7" t="s"/>
+      <c r="G32" s="7" t="s"/>
+      <c r="H32" s="4" t="s"/>
+      <c r="I32" s="25" t="s"/>
+      <c r="J32" s="25" t="s"/>
+      <c r="K32" s="25" t="s"/>
+      <c r="L32" s="7" t="s"/>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="A33" s="4" t="s"/>
+      <c r="B33" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="C33" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D32" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="E32" s="13" t="s"/>
-      <c r="F32" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="G32" s="9" t="s">
+      <c r="D33" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="E33" s="13" t="s"/>
+      <c r="F33" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="G33" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="H32" s="4" t="s"/>
-      <c r="I32" s="24" t="s"/>
-      <c r="J32" s="24" t="s"/>
-      <c r="K32" s="24" t="s"/>
-      <c r="L32" s="7" t="s"/>
-    </row>
-    <row r="33" spans="2:12">
-      <c r="B33" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C33" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="D33" s="33" t="s"/>
-      <c r="E33" s="7" t="s"/>
-      <c r="F33" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="G33" s="40">
-        <v>5744.35</v>
-      </c>
       <c r="H33" s="4" t="s"/>
-      <c r="L33" s="40" t="s"/>
-    </row>
-    <row r="34" spans="2:12" ht="18" customHeight="true">
+      <c r="I33" s="25" t="s"/>
+      <c r="J33" s="25" t="s"/>
+      <c r="K33" s="25" t="s"/>
+      <c r="L33" s="7" t="s"/>
+    </row>
+    <row r="34" spans="2:12">
       <c r="B34" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C34" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="D34" s="33" t="s"/>
+      <c r="C34" s="43" t="s">
+        <v>41</v>
+      </c>
+      <c r="D34" s="34" t="s"/>
       <c r="E34" s="7" t="s"/>
-      <c r="F34" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="G34" s="40">
-        <v>1423.51</v>
+      <c r="F34" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="G34" s="44">
+        <v>5744.35</v>
       </c>
       <c r="H34" s="4" t="s"/>
-      <c r="L34" s="40" t="s"/>
-    </row>
-    <row r="35" spans="2:12">
+      <c r="L34" s="44" t="s"/>
+    </row>
+    <row r="35" spans="2:12" ht="18" customHeight="true">
       <c r="B35" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C35" s="39" t="s">
-        <v>55</v>
-      </c>
-      <c r="D35" s="33" t="s"/>
+      <c r="C35" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="D35" s="34" t="s"/>
       <c r="E35" s="7" t="s"/>
-      <c r="F35" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="G35" s="40">
-        <v>2072.17</v>
+      <c r="F35" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="G35" s="44">
+        <v>1423.51</v>
       </c>
       <c r="H35" s="4" t="s"/>
-      <c r="L35" s="40" t="s"/>
-    </row>
-    <row r="36" spans="2:12" ht="18" customHeight="true">
+      <c r="L35" s="44" t="s"/>
+    </row>
+    <row r="36" spans="2:12">
       <c r="B36" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C36" s="39" t="s">
-        <v>93</v>
-      </c>
-      <c r="D36" s="33" t="s"/>
+      <c r="C36" s="43" t="s">
+        <v>56</v>
+      </c>
+      <c r="D36" s="34" t="s"/>
       <c r="E36" s="7" t="s"/>
-      <c r="F36" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="G36" s="40">
-        <v>2787.55</v>
+      <c r="F36" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="G36" s="44">
+        <v>2072.17</v>
       </c>
       <c r="H36" s="4" t="s"/>
-      <c r="L36" s="40" t="s"/>
+      <c r="L36" s="44" t="s"/>
     </row>
     <row r="37" spans="2:12" ht="18" customHeight="true">
       <c r="B37" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C37" s="39" t="s">
-        <v>93</v>
-      </c>
-      <c r="D37" s="33" t="s"/>
+      <c r="C37" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="D37" s="34" t="s"/>
       <c r="E37" s="7" t="s"/>
-      <c r="F37" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="G37" s="40">
+      <c r="F37" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="G37" s="44">
+        <v>2787.55</v>
+      </c>
+      <c r="H37" s="4" t="s"/>
+      <c r="L37" s="44" t="s"/>
+    </row>
+    <row r="38" spans="2:12" ht="18" customHeight="true">
+      <c r="B38" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="D38" s="34" t="s"/>
+      <c r="E38" s="7" t="s"/>
+      <c r="F38" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="G38" s="44">
         <v>929.23</v>
       </c>
-      <c r="H37" s="4" t="s"/>
-      <c r="L37" s="40" t="s"/>
-    </row>
-    <row r="38" spans="1:12" ht="18" customHeight="true">
-      <c r="A38" s="6" t="s"/>
-      <c r="B38" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D38" s="33" t="s"/>
-      <c r="E38" s="7" t="s"/>
-      <c r="F38" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="G38" s="40">
+      <c r="H38" s="4" t="s"/>
+      <c r="L38" s="44" t="s"/>
+    </row>
+    <row r="39" spans="1:12" ht="18" customHeight="true">
+      <c r="A39" s="6" t="s"/>
+      <c r="B39" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D39" s="34" t="s"/>
+      <c r="E39" s="7" t="s"/>
+      <c r="F39" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="G39" s="44">
         <v>1626.94</v>
       </c>
-      <c r="H38" s="4" t="s"/>
-      <c r="L38" s="40" t="s"/>
-    </row>
-    <row r="39" spans="1:12">
-      <c r="A39" s="4" t="s"/>
-      <c r="B39" s="4" t="s"/>
-      <c r="C39" s="4" t="s"/>
-      <c r="D39" s="4" t="s"/>
-      <c r="E39" s="7" t="s"/>
-      <c r="F39" s="7" t="s"/>
-      <c r="G39" s="7" t="s"/>
       <c r="H39" s="4" t="s"/>
-      <c r="I39" s="24" t="s"/>
-      <c r="J39" s="24" t="s"/>
-      <c r="K39" s="24" t="s"/>
-      <c r="L39" s="7" t="s"/>
+      <c r="L39" s="44" t="s"/>
     </row>
     <row r="40" spans="1:12">
       <c r="A40" s="4" t="s"/>
@@ -1773,9 +1858,9 @@
       <c r="F40" s="7" t="s"/>
       <c r="G40" s="7" t="s"/>
       <c r="H40" s="4" t="s"/>
-      <c r="I40" s="24" t="s"/>
-      <c r="J40" s="24" t="s"/>
-      <c r="K40" s="24" t="s"/>
+      <c r="I40" s="25" t="s"/>
+      <c r="J40" s="25" t="s"/>
+      <c r="K40" s="25" t="s"/>
       <c r="L40" s="7" t="s"/>
     </row>
     <row r="41" spans="1:12">
@@ -1787,9 +1872,9 @@
       <c r="F41" s="7" t="s"/>
       <c r="G41" s="7" t="s"/>
       <c r="H41" s="4" t="s"/>
-      <c r="I41" s="24" t="s"/>
-      <c r="J41" s="24" t="s"/>
-      <c r="K41" s="24" t="s"/>
+      <c r="I41" s="25" t="s"/>
+      <c r="J41" s="25" t="s"/>
+      <c r="K41" s="25" t="s"/>
       <c r="L41" s="7" t="s"/>
     </row>
     <row r="42" spans="1:12">
@@ -1801,9 +1886,9 @@
       <c r="F42" s="7" t="s"/>
       <c r="G42" s="7" t="s"/>
       <c r="H42" s="4" t="s"/>
-      <c r="I42" s="24" t="s"/>
-      <c r="J42" s="24" t="s"/>
-      <c r="K42" s="24" t="s"/>
+      <c r="I42" s="25" t="s"/>
+      <c r="J42" s="25" t="s"/>
+      <c r="K42" s="25" t="s"/>
       <c r="L42" s="7" t="s"/>
     </row>
     <row r="43" spans="1:12">
@@ -1815,9 +1900,9 @@
       <c r="F43" s="7" t="s"/>
       <c r="G43" s="7" t="s"/>
       <c r="H43" s="4" t="s"/>
-      <c r="I43" s="24" t="s"/>
-      <c r="J43" s="24" t="s"/>
-      <c r="K43" s="24" t="s"/>
+      <c r="I43" s="25" t="s"/>
+      <c r="J43" s="25" t="s"/>
+      <c r="K43" s="25" t="s"/>
       <c r="L43" s="7" t="s"/>
     </row>
     <row r="44" spans="1:12">
@@ -1829,9 +1914,9 @@
       <c r="F44" s="7" t="s"/>
       <c r="G44" s="7" t="s"/>
       <c r="H44" s="4" t="s"/>
-      <c r="I44" s="24" t="s"/>
-      <c r="J44" s="24" t="s"/>
-      <c r="K44" s="24" t="s"/>
+      <c r="I44" s="25" t="s"/>
+      <c r="J44" s="25" t="s"/>
+      <c r="K44" s="25" t="s"/>
       <c r="L44" s="7" t="s"/>
     </row>
     <row r="45" spans="1:12">
@@ -1843,9 +1928,9 @@
       <c r="F45" s="7" t="s"/>
       <c r="G45" s="7" t="s"/>
       <c r="H45" s="4" t="s"/>
-      <c r="I45" s="24" t="s"/>
-      <c r="J45" s="24" t="s"/>
-      <c r="K45" s="24" t="s"/>
+      <c r="I45" s="25" t="s"/>
+      <c r="J45" s="25" t="s"/>
+      <c r="K45" s="25" t="s"/>
       <c r="L45" s="7" t="s"/>
     </row>
     <row r="46" spans="1:12">
@@ -1857,9 +1942,9 @@
       <c r="F46" s="7" t="s"/>
       <c r="G46" s="7" t="s"/>
       <c r="H46" s="4" t="s"/>
-      <c r="I46" s="24" t="s"/>
-      <c r="J46" s="24" t="s"/>
-      <c r="K46" s="24" t="s"/>
+      <c r="I46" s="25" t="s"/>
+      <c r="J46" s="25" t="s"/>
+      <c r="K46" s="25" t="s"/>
       <c r="L46" s="7" t="s"/>
     </row>
     <row r="47" spans="1:12">
@@ -1871,9 +1956,9 @@
       <c r="F47" s="7" t="s"/>
       <c r="G47" s="7" t="s"/>
       <c r="H47" s="4" t="s"/>
-      <c r="I47" s="24" t="s"/>
-      <c r="J47" s="24" t="s"/>
-      <c r="K47" s="24" t="s"/>
+      <c r="I47" s="25" t="s"/>
+      <c r="J47" s="25" t="s"/>
+      <c r="K47" s="25" t="s"/>
       <c r="L47" s="7" t="s"/>
     </row>
     <row r="48" spans="1:12">
@@ -1885,9 +1970,9 @@
       <c r="F48" s="7" t="s"/>
       <c r="G48" s="7" t="s"/>
       <c r="H48" s="4" t="s"/>
-      <c r="I48" s="24" t="s"/>
-      <c r="J48" s="24" t="s"/>
-      <c r="K48" s="24" t="s"/>
+      <c r="I48" s="25" t="s"/>
+      <c r="J48" s="25" t="s"/>
+      <c r="K48" s="25" t="s"/>
       <c r="L48" s="7" t="s"/>
     </row>
     <row r="49" spans="1:12">
@@ -1899,9 +1984,9 @@
       <c r="F49" s="7" t="s"/>
       <c r="G49" s="7" t="s"/>
       <c r="H49" s="4" t="s"/>
-      <c r="I49" s="24" t="s"/>
-      <c r="J49" s="24" t="s"/>
-      <c r="K49" s="24" t="s"/>
+      <c r="I49" s="25" t="s"/>
+      <c r="J49" s="25" t="s"/>
+      <c r="K49" s="25" t="s"/>
       <c r="L49" s="7" t="s"/>
     </row>
     <row r="50" spans="1:12">
@@ -1913,9 +1998,9 @@
       <c r="F50" s="7" t="s"/>
       <c r="G50" s="7" t="s"/>
       <c r="H50" s="4" t="s"/>
-      <c r="I50" s="24" t="s"/>
-      <c r="J50" s="24" t="s"/>
-      <c r="K50" s="24" t="s"/>
+      <c r="I50" s="25" t="s"/>
+      <c r="J50" s="25" t="s"/>
+      <c r="K50" s="25" t="s"/>
       <c r="L50" s="7" t="s"/>
     </row>
     <row r="51" spans="1:12">
@@ -1927,9 +2012,9 @@
       <c r="F51" s="7" t="s"/>
       <c r="G51" s="7" t="s"/>
       <c r="H51" s="4" t="s"/>
-      <c r="I51" s="24" t="s"/>
-      <c r="J51" s="24" t="s"/>
-      <c r="K51" s="24" t="s"/>
+      <c r="I51" s="25" t="s"/>
+      <c r="J51" s="25" t="s"/>
+      <c r="K51" s="25" t="s"/>
       <c r="L51" s="7" t="s"/>
     </row>
     <row r="52" spans="1:12">
@@ -1941,9 +2026,9 @@
       <c r="F52" s="7" t="s"/>
       <c r="G52" s="7" t="s"/>
       <c r="H52" s="4" t="s"/>
-      <c r="I52" s="24" t="s"/>
-      <c r="J52" s="24" t="s"/>
-      <c r="K52" s="24" t="s"/>
+      <c r="I52" s="25" t="s"/>
+      <c r="J52" s="25" t="s"/>
+      <c r="K52" s="25" t="s"/>
       <c r="L52" s="7" t="s"/>
     </row>
     <row r="53" spans="1:12">
@@ -1955,9 +2040,9 @@
       <c r="F53" s="7" t="s"/>
       <c r="G53" s="7" t="s"/>
       <c r="H53" s="4" t="s"/>
-      <c r="I53" s="24" t="s"/>
-      <c r="J53" s="24" t="s"/>
-      <c r="K53" s="24" t="s"/>
+      <c r="I53" s="25" t="s"/>
+      <c r="J53" s="25" t="s"/>
+      <c r="K53" s="25" t="s"/>
       <c r="L53" s="7" t="s"/>
     </row>
     <row r="54" spans="1:12">
@@ -1969,9 +2054,9 @@
       <c r="F54" s="7" t="s"/>
       <c r="G54" s="7" t="s"/>
       <c r="H54" s="4" t="s"/>
-      <c r="I54" s="24" t="s"/>
-      <c r="J54" s="24" t="s"/>
-      <c r="K54" s="24" t="s"/>
+      <c r="I54" s="25" t="s"/>
+      <c r="J54" s="25" t="s"/>
+      <c r="K54" s="25" t="s"/>
       <c r="L54" s="7" t="s"/>
     </row>
     <row r="55" spans="1:12">
@@ -1983,9 +2068,9 @@
       <c r="F55" s="7" t="s"/>
       <c r="G55" s="7" t="s"/>
       <c r="H55" s="4" t="s"/>
-      <c r="I55" s="24" t="s"/>
-      <c r="J55" s="24" t="s"/>
-      <c r="K55" s="24" t="s"/>
+      <c r="I55" s="25" t="s"/>
+      <c r="J55" s="25" t="s"/>
+      <c r="K55" s="25" t="s"/>
       <c r="L55" s="7" t="s"/>
     </row>
     <row r="56" spans="1:12">
@@ -1997,9 +2082,9 @@
       <c r="F56" s="7" t="s"/>
       <c r="G56" s="7" t="s"/>
       <c r="H56" s="4" t="s"/>
-      <c r="I56" s="24" t="s"/>
-      <c r="J56" s="24" t="s"/>
-      <c r="K56" s="24" t="s"/>
+      <c r="I56" s="25" t="s"/>
+      <c r="J56" s="25" t="s"/>
+      <c r="K56" s="25" t="s"/>
       <c r="L56" s="7" t="s"/>
     </row>
     <row r="57" spans="1:12">
@@ -2011,9 +2096,9 @@
       <c r="F57" s="7" t="s"/>
       <c r="G57" s="7" t="s"/>
       <c r="H57" s="4" t="s"/>
-      <c r="I57" s="24" t="s"/>
-      <c r="J57" s="24" t="s"/>
-      <c r="K57" s="24" t="s"/>
+      <c r="I57" s="25" t="s"/>
+      <c r="J57" s="25" t="s"/>
+      <c r="K57" s="25" t="s"/>
       <c r="L57" s="7" t="s"/>
     </row>
     <row r="58" spans="1:12">
@@ -2025,9 +2110,9 @@
       <c r="F58" s="7" t="s"/>
       <c r="G58" s="7" t="s"/>
       <c r="H58" s="4" t="s"/>
-      <c r="I58" s="24" t="s"/>
-      <c r="J58" s="24" t="s"/>
-      <c r="K58" s="24" t="s"/>
+      <c r="I58" s="25" t="s"/>
+      <c r="J58" s="25" t="s"/>
+      <c r="K58" s="25" t="s"/>
       <c r="L58" s="7" t="s"/>
     </row>
     <row r="59" spans="1:12">
@@ -2039,9 +2124,9 @@
       <c r="F59" s="7" t="s"/>
       <c r="G59" s="7" t="s"/>
       <c r="H59" s="4" t="s"/>
-      <c r="I59" s="24" t="s"/>
-      <c r="J59" s="24" t="s"/>
-      <c r="K59" s="24" t="s"/>
+      <c r="I59" s="25" t="s"/>
+      <c r="J59" s="25" t="s"/>
+      <c r="K59" s="25" t="s"/>
       <c r="L59" s="7" t="s"/>
     </row>
     <row r="60" spans="1:12">
@@ -2053,9 +2138,9 @@
       <c r="F60" s="7" t="s"/>
       <c r="G60" s="7" t="s"/>
       <c r="H60" s="4" t="s"/>
-      <c r="I60" s="24" t="s"/>
-      <c r="J60" s="24" t="s"/>
-      <c r="K60" s="24" t="s"/>
+      <c r="I60" s="25" t="s"/>
+      <c r="J60" s="25" t="s"/>
+      <c r="K60" s="25" t="s"/>
       <c r="L60" s="7" t="s"/>
     </row>
     <row r="61" spans="1:12">
@@ -2067,9 +2152,9 @@
       <c r="F61" s="7" t="s"/>
       <c r="G61" s="7" t="s"/>
       <c r="H61" s="4" t="s"/>
-      <c r="I61" s="24" t="s"/>
-      <c r="J61" s="24" t="s"/>
-      <c r="K61" s="24" t="s"/>
+      <c r="I61" s="25" t="s"/>
+      <c r="J61" s="25" t="s"/>
+      <c r="K61" s="25" t="s"/>
       <c r="L61" s="7" t="s"/>
     </row>
     <row r="62" spans="1:12">
@@ -2081,9 +2166,9 @@
       <c r="F62" s="7" t="s"/>
       <c r="G62" s="7" t="s"/>
       <c r="H62" s="4" t="s"/>
-      <c r="I62" s="24" t="s"/>
-      <c r="J62" s="24" t="s"/>
-      <c r="K62" s="24" t="s"/>
+      <c r="I62" s="25" t="s"/>
+      <c r="J62" s="25" t="s"/>
+      <c r="K62" s="25" t="s"/>
       <c r="L62" s="7" t="s"/>
     </row>
     <row r="63" spans="1:12">
@@ -2095,9 +2180,9 @@
       <c r="F63" s="7" t="s"/>
       <c r="G63" s="7" t="s"/>
       <c r="H63" s="4" t="s"/>
-      <c r="I63" s="24" t="s"/>
-      <c r="J63" s="24" t="s"/>
-      <c r="K63" s="24" t="s"/>
+      <c r="I63" s="25" t="s"/>
+      <c r="J63" s="25" t="s"/>
+      <c r="K63" s="25" t="s"/>
       <c r="L63" s="7" t="s"/>
     </row>
     <row r="64" spans="1:12">
@@ -2109,9 +2194,9 @@
       <c r="F64" s="7" t="s"/>
       <c r="G64" s="7" t="s"/>
       <c r="H64" s="4" t="s"/>
-      <c r="I64" s="24" t="s"/>
-      <c r="J64" s="24" t="s"/>
-      <c r="K64" s="24" t="s"/>
+      <c r="I64" s="25" t="s"/>
+      <c r="J64" s="25" t="s"/>
+      <c r="K64" s="25" t="s"/>
       <c r="L64" s="7" t="s"/>
     </row>
     <row r="65" spans="1:12">
@@ -2123,9 +2208,9 @@
       <c r="F65" s="7" t="s"/>
       <c r="G65" s="7" t="s"/>
       <c r="H65" s="4" t="s"/>
-      <c r="I65" s="24" t="s"/>
-      <c r="J65" s="24" t="s"/>
-      <c r="K65" s="24" t="s"/>
+      <c r="I65" s="25" t="s"/>
+      <c r="J65" s="25" t="s"/>
+      <c r="K65" s="25" t="s"/>
       <c r="L65" s="7" t="s"/>
     </row>
     <row r="66" spans="1:12">
@@ -2137,9 +2222,9 @@
       <c r="F66" s="7" t="s"/>
       <c r="G66" s="7" t="s"/>
       <c r="H66" s="4" t="s"/>
-      <c r="I66" s="24" t="s"/>
-      <c r="J66" s="24" t="s"/>
-      <c r="K66" s="24" t="s"/>
+      <c r="I66" s="25" t="s"/>
+      <c r="J66" s="25" t="s"/>
+      <c r="K66" s="25" t="s"/>
       <c r="L66" s="7" t="s"/>
     </row>
     <row r="67" spans="1:12">
@@ -2151,9 +2236,9 @@
       <c r="F67" s="7" t="s"/>
       <c r="G67" s="7" t="s"/>
       <c r="H67" s="4" t="s"/>
-      <c r="I67" s="24" t="s"/>
-      <c r="J67" s="24" t="s"/>
-      <c r="K67" s="24" t="s"/>
+      <c r="I67" s="25" t="s"/>
+      <c r="J67" s="25" t="s"/>
+      <c r="K67" s="25" t="s"/>
       <c r="L67" s="7" t="s"/>
     </row>
     <row r="68" spans="1:12">
@@ -2165,9 +2250,9 @@
       <c r="F68" s="7" t="s"/>
       <c r="G68" s="7" t="s"/>
       <c r="H68" s="4" t="s"/>
-      <c r="I68" s="24" t="s"/>
-      <c r="J68" s="24" t="s"/>
-      <c r="K68" s="24" t="s"/>
+      <c r="I68" s="25" t="s"/>
+      <c r="J68" s="25" t="s"/>
+      <c r="K68" s="25" t="s"/>
       <c r="L68" s="7" t="s"/>
     </row>
     <row r="69" spans="1:12">
@@ -2179,9 +2264,9 @@
       <c r="F69" s="7" t="s"/>
       <c r="G69" s="7" t="s"/>
       <c r="H69" s="4" t="s"/>
-      <c r="I69" s="24" t="s"/>
-      <c r="J69" s="24" t="s"/>
-      <c r="K69" s="24" t="s"/>
+      <c r="I69" s="25" t="s"/>
+      <c r="J69" s="25" t="s"/>
+      <c r="K69" s="25" t="s"/>
       <c r="L69" s="7" t="s"/>
     </row>
     <row r="70" spans="1:12">
@@ -2193,9 +2278,9 @@
       <c r="F70" s="7" t="s"/>
       <c r="G70" s="7" t="s"/>
       <c r="H70" s="4" t="s"/>
-      <c r="I70" s="24" t="s"/>
-      <c r="J70" s="24" t="s"/>
-      <c r="K70" s="24" t="s"/>
+      <c r="I70" s="25" t="s"/>
+      <c r="J70" s="25" t="s"/>
+      <c r="K70" s="25" t="s"/>
       <c r="L70" s="7" t="s"/>
     </row>
     <row r="71" spans="1:12">
@@ -2207,9 +2292,9 @@
       <c r="F71" s="7" t="s"/>
       <c r="G71" s="7" t="s"/>
       <c r="H71" s="4" t="s"/>
-      <c r="I71" s="24" t="s"/>
-      <c r="J71" s="24" t="s"/>
-      <c r="K71" s="24" t="s"/>
+      <c r="I71" s="25" t="s"/>
+      <c r="J71" s="25" t="s"/>
+      <c r="K71" s="25" t="s"/>
       <c r="L71" s="7" t="s"/>
     </row>
     <row r="72" spans="1:12">
@@ -2221,9 +2306,9 @@
       <c r="F72" s="7" t="s"/>
       <c r="G72" s="7" t="s"/>
       <c r="H72" s="4" t="s"/>
-      <c r="I72" s="24" t="s"/>
-      <c r="J72" s="24" t="s"/>
-      <c r="K72" s="24" t="s"/>
+      <c r="I72" s="25" t="s"/>
+      <c r="J72" s="25" t="s"/>
+      <c r="K72" s="25" t="s"/>
       <c r="L72" s="7" t="s"/>
     </row>
     <row r="73" spans="1:12">
@@ -2235,9 +2320,9 @@
       <c r="F73" s="7" t="s"/>
       <c r="G73" s="7" t="s"/>
       <c r="H73" s="4" t="s"/>
-      <c r="I73" s="24" t="s"/>
-      <c r="J73" s="24" t="s"/>
-      <c r="K73" s="24" t="s"/>
+      <c r="I73" s="25" t="s"/>
+      <c r="J73" s="25" t="s"/>
+      <c r="K73" s="25" t="s"/>
       <c r="L73" s="7" t="s"/>
     </row>
     <row r="74" spans="1:12">
@@ -2249,9 +2334,9 @@
       <c r="F74" s="7" t="s"/>
       <c r="G74" s="7" t="s"/>
       <c r="H74" s="4" t="s"/>
-      <c r="I74" s="24" t="s"/>
-      <c r="J74" s="24" t="s"/>
-      <c r="K74" s="24" t="s"/>
+      <c r="I74" s="25" t="s"/>
+      <c r="J74" s="25" t="s"/>
+      <c r="K74" s="25" t="s"/>
       <c r="L74" s="7" t="s"/>
     </row>
     <row r="75" spans="1:12">
@@ -2263,9 +2348,9 @@
       <c r="F75" s="7" t="s"/>
       <c r="G75" s="7" t="s"/>
       <c r="H75" s="4" t="s"/>
-      <c r="I75" s="24" t="s"/>
-      <c r="J75" s="24" t="s"/>
-      <c r="K75" s="24" t="s"/>
+      <c r="I75" s="25" t="s"/>
+      <c r="J75" s="25" t="s"/>
+      <c r="K75" s="25" t="s"/>
       <c r="L75" s="7" t="s"/>
     </row>
     <row r="76" spans="1:12">
@@ -2277,9 +2362,9 @@
       <c r="F76" s="7" t="s"/>
       <c r="G76" s="7" t="s"/>
       <c r="H76" s="4" t="s"/>
-      <c r="I76" s="24" t="s"/>
-      <c r="J76" s="24" t="s"/>
-      <c r="K76" s="24" t="s"/>
+      <c r="I76" s="25" t="s"/>
+      <c r="J76" s="25" t="s"/>
+      <c r="K76" s="25" t="s"/>
       <c r="L76" s="7" t="s"/>
     </row>
     <row r="77" spans="1:12">
@@ -2291,9 +2376,9 @@
       <c r="F77" s="7" t="s"/>
       <c r="G77" s="7" t="s"/>
       <c r="H77" s="4" t="s"/>
-      <c r="I77" s="24" t="s"/>
-      <c r="J77" s="24" t="s"/>
-      <c r="K77" s="24" t="s"/>
+      <c r="I77" s="25" t="s"/>
+      <c r="J77" s="25" t="s"/>
+      <c r="K77" s="25" t="s"/>
       <c r="L77" s="7" t="s"/>
     </row>
     <row r="78" spans="1:12">
@@ -2305,9 +2390,9 @@
       <c r="F78" s="7" t="s"/>
       <c r="G78" s="7" t="s"/>
       <c r="H78" s="4" t="s"/>
-      <c r="I78" s="24" t="s"/>
-      <c r="J78" s="24" t="s"/>
-      <c r="K78" s="24" t="s"/>
+      <c r="I78" s="25" t="s"/>
+      <c r="J78" s="25" t="s"/>
+      <c r="K78" s="25" t="s"/>
       <c r="L78" s="7" t="s"/>
     </row>
     <row r="79" spans="1:12">
@@ -2319,9 +2404,9 @@
       <c r="F79" s="7" t="s"/>
       <c r="G79" s="7" t="s"/>
       <c r="H79" s="4" t="s"/>
-      <c r="I79" s="24" t="s"/>
-      <c r="J79" s="24" t="s"/>
-      <c r="K79" s="24" t="s"/>
+      <c r="I79" s="25" t="s"/>
+      <c r="J79" s="25" t="s"/>
+      <c r="K79" s="25" t="s"/>
       <c r="L79" s="7" t="s"/>
     </row>
     <row r="80" spans="1:12">
@@ -2333,9 +2418,9 @@
       <c r="F80" s="7" t="s"/>
       <c r="G80" s="7" t="s"/>
       <c r="H80" s="4" t="s"/>
-      <c r="I80" s="24" t="s"/>
-      <c r="J80" s="24" t="s"/>
-      <c r="K80" s="24" t="s"/>
+      <c r="I80" s="25" t="s"/>
+      <c r="J80" s="25" t="s"/>
+      <c r="K80" s="25" t="s"/>
       <c r="L80" s="7" t="s"/>
     </row>
     <row r="81" spans="1:12">
@@ -2347,9 +2432,9 @@
       <c r="F81" s="7" t="s"/>
       <c r="G81" s="7" t="s"/>
       <c r="H81" s="4" t="s"/>
-      <c r="I81" s="24" t="s"/>
-      <c r="J81" s="24" t="s"/>
-      <c r="K81" s="24" t="s"/>
+      <c r="I81" s="25" t="s"/>
+      <c r="J81" s="25" t="s"/>
+      <c r="K81" s="25" t="s"/>
       <c r="L81" s="7" t="s"/>
     </row>
     <row r="82" spans="1:12">
@@ -2361,9 +2446,9 @@
       <c r="F82" s="7" t="s"/>
       <c r="G82" s="7" t="s"/>
       <c r="H82" s="4" t="s"/>
-      <c r="I82" s="24" t="s"/>
-      <c r="J82" s="24" t="s"/>
-      <c r="K82" s="24" t="s"/>
+      <c r="I82" s="25" t="s"/>
+      <c r="J82" s="25" t="s"/>
+      <c r="K82" s="25" t="s"/>
       <c r="L82" s="7" t="s"/>
     </row>
     <row r="83" spans="1:12">
@@ -2375,9 +2460,9 @@
       <c r="F83" s="7" t="s"/>
       <c r="G83" s="7" t="s"/>
       <c r="H83" s="4" t="s"/>
-      <c r="I83" s="24" t="s"/>
-      <c r="J83" s="24" t="s"/>
-      <c r="K83" s="24" t="s"/>
+      <c r="I83" s="25" t="s"/>
+      <c r="J83" s="25" t="s"/>
+      <c r="K83" s="25" t="s"/>
       <c r="L83" s="7" t="s"/>
     </row>
     <row r="84" spans="1:12">
@@ -2389,9 +2474,9 @@
       <c r="F84" s="7" t="s"/>
       <c r="G84" s="7" t="s"/>
       <c r="H84" s="4" t="s"/>
-      <c r="I84" s="24" t="s"/>
-      <c r="J84" s="24" t="s"/>
-      <c r="K84" s="24" t="s"/>
+      <c r="I84" s="25" t="s"/>
+      <c r="J84" s="25" t="s"/>
+      <c r="K84" s="25" t="s"/>
       <c r="L84" s="7" t="s"/>
     </row>
     <row r="85" spans="1:12">
@@ -2403,9 +2488,9 @@
       <c r="F85" s="7" t="s"/>
       <c r="G85" s="7" t="s"/>
       <c r="H85" s="4" t="s"/>
-      <c r="I85" s="24" t="s"/>
-      <c r="J85" s="24" t="s"/>
-      <c r="K85" s="24" t="s"/>
+      <c r="I85" s="25" t="s"/>
+      <c r="J85" s="25" t="s"/>
+      <c r="K85" s="25" t="s"/>
       <c r="L85" s="7" t="s"/>
     </row>
     <row r="86" spans="1:12">
@@ -2417,9 +2502,9 @@
       <c r="F86" s="7" t="s"/>
       <c r="G86" s="7" t="s"/>
       <c r="H86" s="4" t="s"/>
-      <c r="I86" s="24" t="s"/>
-      <c r="J86" s="24" t="s"/>
-      <c r="K86" s="24" t="s"/>
+      <c r="I86" s="25" t="s"/>
+      <c r="J86" s="25" t="s"/>
+      <c r="K86" s="25" t="s"/>
       <c r="L86" s="7" t="s"/>
     </row>
     <row r="87" spans="1:12">
@@ -2431,9 +2516,9 @@
       <c r="F87" s="7" t="s"/>
       <c r="G87" s="7" t="s"/>
       <c r="H87" s="4" t="s"/>
-      <c r="I87" s="24" t="s"/>
-      <c r="J87" s="24" t="s"/>
-      <c r="K87" s="24" t="s"/>
+      <c r="I87" s="25" t="s"/>
+      <c r="J87" s="25" t="s"/>
+      <c r="K87" s="25" t="s"/>
       <c r="L87" s="7" t="s"/>
     </row>
     <row r="88" spans="1:12">
@@ -2445,9 +2530,9 @@
       <c r="F88" s="7" t="s"/>
       <c r="G88" s="7" t="s"/>
       <c r="H88" s="4" t="s"/>
-      <c r="I88" s="24" t="s"/>
-      <c r="J88" s="24" t="s"/>
-      <c r="K88" s="24" t="s"/>
+      <c r="I88" s="25" t="s"/>
+      <c r="J88" s="25" t="s"/>
+      <c r="K88" s="25" t="s"/>
       <c r="L88" s="7" t="s"/>
     </row>
     <row r="89" spans="1:12">
@@ -2459,9 +2544,9 @@
       <c r="F89" s="7" t="s"/>
       <c r="G89" s="7" t="s"/>
       <c r="H89" s="4" t="s"/>
-      <c r="I89" s="24" t="s"/>
-      <c r="J89" s="24" t="s"/>
-      <c r="K89" s="24" t="s"/>
+      <c r="I89" s="25" t="s"/>
+      <c r="J89" s="25" t="s"/>
+      <c r="K89" s="25" t="s"/>
       <c r="L89" s="7" t="s"/>
     </row>
     <row r="90" spans="1:12">
@@ -2473,9 +2558,9 @@
       <c r="F90" s="7" t="s"/>
       <c r="G90" s="7" t="s"/>
       <c r="H90" s="4" t="s"/>
-      <c r="I90" s="24" t="s"/>
-      <c r="J90" s="24" t="s"/>
-      <c r="K90" s="24" t="s"/>
+      <c r="I90" s="25" t="s"/>
+      <c r="J90" s="25" t="s"/>
+      <c r="K90" s="25" t="s"/>
       <c r="L90" s="7" t="s"/>
     </row>
     <row r="91" spans="1:12">
@@ -2487,9 +2572,9 @@
       <c r="F91" s="7" t="s"/>
       <c r="G91" s="7" t="s"/>
       <c r="H91" s="4" t="s"/>
-      <c r="I91" s="24" t="s"/>
-      <c r="J91" s="24" t="s"/>
-      <c r="K91" s="24" t="s"/>
+      <c r="I91" s="25" t="s"/>
+      <c r="J91" s="25" t="s"/>
+      <c r="K91" s="25" t="s"/>
       <c r="L91" s="7" t="s"/>
     </row>
     <row r="92" spans="1:12">
@@ -2501,9 +2586,9 @@
       <c r="F92" s="7" t="s"/>
       <c r="G92" s="7" t="s"/>
       <c r="H92" s="4" t="s"/>
-      <c r="I92" s="24" t="s"/>
-      <c r="J92" s="24" t="s"/>
-      <c r="K92" s="24" t="s"/>
+      <c r="I92" s="25" t="s"/>
+      <c r="J92" s="25" t="s"/>
+      <c r="K92" s="25" t="s"/>
       <c r="L92" s="7" t="s"/>
     </row>
     <row r="93" spans="1:12">
@@ -2515,9 +2600,9 @@
       <c r="F93" s="7" t="s"/>
       <c r="G93" s="7" t="s"/>
       <c r="H93" s="4" t="s"/>
-      <c r="I93" s="24" t="s"/>
-      <c r="J93" s="24" t="s"/>
-      <c r="K93" s="24" t="s"/>
+      <c r="I93" s="25" t="s"/>
+      <c r="J93" s="25" t="s"/>
+      <c r="K93" s="25" t="s"/>
       <c r="L93" s="7" t="s"/>
     </row>
     <row r="94" spans="1:12">
@@ -2529,9 +2614,9 @@
       <c r="F94" s="7" t="s"/>
       <c r="G94" s="7" t="s"/>
       <c r="H94" s="4" t="s"/>
-      <c r="I94" s="24" t="s"/>
-      <c r="J94" s="24" t="s"/>
-      <c r="K94" s="24" t="s"/>
+      <c r="I94" s="25" t="s"/>
+      <c r="J94" s="25" t="s"/>
+      <c r="K94" s="25" t="s"/>
       <c r="L94" s="7" t="s"/>
     </row>
     <row r="95" spans="1:12">
@@ -2543,9 +2628,9 @@
       <c r="F95" s="7" t="s"/>
       <c r="G95" s="7" t="s"/>
       <c r="H95" s="4" t="s"/>
-      <c r="I95" s="24" t="s"/>
-      <c r="J95" s="24" t="s"/>
-      <c r="K95" s="24" t="s"/>
+      <c r="I95" s="25" t="s"/>
+      <c r="J95" s="25" t="s"/>
+      <c r="K95" s="25" t="s"/>
       <c r="L95" s="7" t="s"/>
     </row>
     <row r="96" spans="1:12">
@@ -2557,9 +2642,9 @@
       <c r="F96" s="7" t="s"/>
       <c r="G96" s="7" t="s"/>
       <c r="H96" s="4" t="s"/>
-      <c r="I96" s="24" t="s"/>
-      <c r="J96" s="24" t="s"/>
-      <c r="K96" s="24" t="s"/>
+      <c r="I96" s="25" t="s"/>
+      <c r="J96" s="25" t="s"/>
+      <c r="K96" s="25" t="s"/>
       <c r="L96" s="7" t="s"/>
     </row>
     <row r="97" spans="1:12">
@@ -2571,9 +2656,9 @@
       <c r="F97" s="7" t="s"/>
       <c r="G97" s="7" t="s"/>
       <c r="H97" s="4" t="s"/>
-      <c r="I97" s="24" t="s"/>
-      <c r="J97" s="24" t="s"/>
-      <c r="K97" s="24" t="s"/>
+      <c r="I97" s="25" t="s"/>
+      <c r="J97" s="25" t="s"/>
+      <c r="K97" s="25" t="s"/>
       <c r="L97" s="7" t="s"/>
     </row>
     <row r="98" spans="1:12">
@@ -2585,9 +2670,9 @@
       <c r="F98" s="7" t="s"/>
       <c r="G98" s="7" t="s"/>
       <c r="H98" s="4" t="s"/>
-      <c r="I98" s="24" t="s"/>
-      <c r="J98" s="24" t="s"/>
-      <c r="K98" s="24" t="s"/>
+      <c r="I98" s="25" t="s"/>
+      <c r="J98" s="25" t="s"/>
+      <c r="K98" s="25" t="s"/>
       <c r="L98" s="7" t="s"/>
     </row>
     <row r="99" spans="1:12">
@@ -2599,9 +2684,9 @@
       <c r="F99" s="7" t="s"/>
       <c r="G99" s="7" t="s"/>
       <c r="H99" s="4" t="s"/>
-      <c r="I99" s="24" t="s"/>
-      <c r="J99" s="24" t="s"/>
-      <c r="K99" s="24" t="s"/>
+      <c r="I99" s="25" t="s"/>
+      <c r="J99" s="25" t="s"/>
+      <c r="K99" s="25" t="s"/>
       <c r="L99" s="7" t="s"/>
     </row>
     <row r="100" spans="1:12">
@@ -2613,9 +2698,9 @@
       <c r="F100" s="7" t="s"/>
       <c r="G100" s="7" t="s"/>
       <c r="H100" s="4" t="s"/>
-      <c r="I100" s="24" t="s"/>
-      <c r="J100" s="24" t="s"/>
-      <c r="K100" s="24" t="s"/>
+      <c r="I100" s="25" t="s"/>
+      <c r="J100" s="25" t="s"/>
+      <c r="K100" s="25" t="s"/>
       <c r="L100" s="7" t="s"/>
     </row>
     <row r="101" spans="1:12">
@@ -2627,9 +2712,9 @@
       <c r="F101" s="7" t="s"/>
       <c r="G101" s="7" t="s"/>
       <c r="H101" s="4" t="s"/>
-      <c r="I101" s="24" t="s"/>
-      <c r="J101" s="24" t="s"/>
-      <c r="K101" s="24" t="s"/>
+      <c r="I101" s="25" t="s"/>
+      <c r="J101" s="25" t="s"/>
+      <c r="K101" s="25" t="s"/>
       <c r="L101" s="7" t="s"/>
     </row>
     <row r="102" spans="1:12">
@@ -2641,9 +2726,9 @@
       <c r="F102" s="7" t="s"/>
       <c r="G102" s="7" t="s"/>
       <c r="H102" s="4" t="s"/>
-      <c r="I102" s="24" t="s"/>
-      <c r="J102" s="24" t="s"/>
-      <c r="K102" s="24" t="s"/>
+      <c r="I102" s="25" t="s"/>
+      <c r="J102" s="25" t="s"/>
+      <c r="K102" s="25" t="s"/>
       <c r="L102" s="7" t="s"/>
     </row>
     <row r="103" spans="1:12">
@@ -2655,9 +2740,9 @@
       <c r="F103" s="7" t="s"/>
       <c r="G103" s="7" t="s"/>
       <c r="H103" s="4" t="s"/>
-      <c r="I103" s="24" t="s"/>
-      <c r="J103" s="24" t="s"/>
-      <c r="K103" s="24" t="s"/>
+      <c r="I103" s="25" t="s"/>
+      <c r="J103" s="25" t="s"/>
+      <c r="K103" s="25" t="s"/>
       <c r="L103" s="7" t="s"/>
     </row>
     <row r="104" spans="1:12">
@@ -2669,9 +2754,9 @@
       <c r="F104" s="7" t="s"/>
       <c r="G104" s="7" t="s"/>
       <c r="H104" s="4" t="s"/>
-      <c r="I104" s="24" t="s"/>
-      <c r="J104" s="24" t="s"/>
-      <c r="K104" s="24" t="s"/>
+      <c r="I104" s="25" t="s"/>
+      <c r="J104" s="25" t="s"/>
+      <c r="K104" s="25" t="s"/>
       <c r="L104" s="7" t="s"/>
     </row>
     <row r="105" spans="1:12">
@@ -2683,9 +2768,9 @@
       <c r="F105" s="7" t="s"/>
       <c r="G105" s="7" t="s"/>
       <c r="H105" s="4" t="s"/>
-      <c r="I105" s="24" t="s"/>
-      <c r="J105" s="24" t="s"/>
-      <c r="K105" s="24" t="s"/>
+      <c r="I105" s="25" t="s"/>
+      <c r="J105" s="25" t="s"/>
+      <c r="K105" s="25" t="s"/>
       <c r="L105" s="7" t="s"/>
     </row>
     <row r="106" spans="1:12">
@@ -2697,9 +2782,9 @@
       <c r="F106" s="7" t="s"/>
       <c r="G106" s="7" t="s"/>
       <c r="H106" s="4" t="s"/>
-      <c r="I106" s="24" t="s"/>
-      <c r="J106" s="24" t="s"/>
-      <c r="K106" s="24" t="s"/>
+      <c r="I106" s="25" t="s"/>
+      <c r="J106" s="25" t="s"/>
+      <c r="K106" s="25" t="s"/>
       <c r="L106" s="7" t="s"/>
     </row>
     <row r="107" spans="1:12">
@@ -2711,9 +2796,9 @@
       <c r="F107" s="7" t="s"/>
       <c r="G107" s="7" t="s"/>
       <c r="H107" s="4" t="s"/>
-      <c r="I107" s="24" t="s"/>
-      <c r="J107" s="24" t="s"/>
-      <c r="K107" s="24" t="s"/>
+      <c r="I107" s="25" t="s"/>
+      <c r="J107" s="25" t="s"/>
+      <c r="K107" s="25" t="s"/>
       <c r="L107" s="7" t="s"/>
     </row>
     <row r="108" spans="1:12">
@@ -2725,9 +2810,9 @@
       <c r="F108" s="7" t="s"/>
       <c r="G108" s="7" t="s"/>
       <c r="H108" s="4" t="s"/>
-      <c r="I108" s="24" t="s"/>
-      <c r="J108" s="24" t="s"/>
-      <c r="K108" s="24" t="s"/>
+      <c r="I108" s="25" t="s"/>
+      <c r="J108" s="25" t="s"/>
+      <c r="K108" s="25" t="s"/>
       <c r="L108" s="7" t="s"/>
     </row>
     <row r="109" spans="1:12">
@@ -2739,9 +2824,9 @@
       <c r="F109" s="7" t="s"/>
       <c r="G109" s="7" t="s"/>
       <c r="H109" s="4" t="s"/>
-      <c r="I109" s="24" t="s"/>
-      <c r="J109" s="24" t="s"/>
-      <c r="K109" s="24" t="s"/>
+      <c r="I109" s="25" t="s"/>
+      <c r="J109" s="25" t="s"/>
+      <c r="K109" s="25" t="s"/>
       <c r="L109" s="7" t="s"/>
     </row>
     <row r="110" spans="1:12">
@@ -2753,9 +2838,9 @@
       <c r="F110" s="7" t="s"/>
       <c r="G110" s="7" t="s"/>
       <c r="H110" s="4" t="s"/>
-      <c r="I110" s="24" t="s"/>
-      <c r="J110" s="24" t="s"/>
-      <c r="K110" s="24" t="s"/>
+      <c r="I110" s="25" t="s"/>
+      <c r="J110" s="25" t="s"/>
+      <c r="K110" s="25" t="s"/>
       <c r="L110" s="7" t="s"/>
     </row>
     <row r="111" spans="1:12">
@@ -2767,9 +2852,9 @@
       <c r="F111" s="7" t="s"/>
       <c r="G111" s="7" t="s"/>
       <c r="H111" s="4" t="s"/>
-      <c r="I111" s="24" t="s"/>
-      <c r="J111" s="24" t="s"/>
-      <c r="K111" s="24" t="s"/>
+      <c r="I111" s="25" t="s"/>
+      <c r="J111" s="25" t="s"/>
+      <c r="K111" s="25" t="s"/>
       <c r="L111" s="7" t="s"/>
     </row>
     <row r="112" spans="1:12">
@@ -2781,9 +2866,9 @@
       <c r="F112" s="7" t="s"/>
       <c r="G112" s="7" t="s"/>
       <c r="H112" s="4" t="s"/>
-      <c r="I112" s="24" t="s"/>
-      <c r="J112" s="24" t="s"/>
-      <c r="K112" s="24" t="s"/>
+      <c r="I112" s="25" t="s"/>
+      <c r="J112" s="25" t="s"/>
+      <c r="K112" s="25" t="s"/>
       <c r="L112" s="7" t="s"/>
     </row>
     <row r="113" spans="1:12">
@@ -2795,9 +2880,9 @@
       <c r="F113" s="7" t="s"/>
       <c r="G113" s="7" t="s"/>
       <c r="H113" s="4" t="s"/>
-      <c r="I113" s="24" t="s"/>
-      <c r="J113" s="24" t="s"/>
-      <c r="K113" s="24" t="s"/>
+      <c r="I113" s="25" t="s"/>
+      <c r="J113" s="25" t="s"/>
+      <c r="K113" s="25" t="s"/>
       <c r="L113" s="7" t="s"/>
     </row>
     <row r="114" spans="1:12">
@@ -2809,9 +2894,9 @@
       <c r="F114" s="7" t="s"/>
       <c r="G114" s="7" t="s"/>
       <c r="H114" s="4" t="s"/>
-      <c r="I114" s="24" t="s"/>
-      <c r="J114" s="24" t="s"/>
-      <c r="K114" s="24" t="s"/>
+      <c r="I114" s="25" t="s"/>
+      <c r="J114" s="25" t="s"/>
+      <c r="K114" s="25" t="s"/>
       <c r="L114" s="7" t="s"/>
     </row>
     <row r="115" spans="1:12">
@@ -2823,9 +2908,9 @@
       <c r="F115" s="7" t="s"/>
       <c r="G115" s="7" t="s"/>
       <c r="H115" s="4" t="s"/>
-      <c r="I115" s="24" t="s"/>
-      <c r="J115" s="24" t="s"/>
-      <c r="K115" s="24" t="s"/>
+      <c r="I115" s="25" t="s"/>
+      <c r="J115" s="25" t="s"/>
+      <c r="K115" s="25" t="s"/>
       <c r="L115" s="7" t="s"/>
     </row>
     <row r="116" spans="1:12">
@@ -2837,9 +2922,9 @@
       <c r="F116" s="7" t="s"/>
       <c r="G116" s="7" t="s"/>
       <c r="H116" s="4" t="s"/>
-      <c r="I116" s="24" t="s"/>
-      <c r="J116" s="24" t="s"/>
-      <c r="K116" s="24" t="s"/>
+      <c r="I116" s="25" t="s"/>
+      <c r="J116" s="25" t="s"/>
+      <c r="K116" s="25" t="s"/>
       <c r="L116" s="7" t="s"/>
     </row>
     <row r="117" spans="1:12">
@@ -2851,9 +2936,9 @@
       <c r="F117" s="7" t="s"/>
       <c r="G117" s="7" t="s"/>
       <c r="H117" s="4" t="s"/>
-      <c r="I117" s="24" t="s"/>
-      <c r="J117" s="24" t="s"/>
-      <c r="K117" s="24" t="s"/>
+      <c r="I117" s="25" t="s"/>
+      <c r="J117" s="25" t="s"/>
+      <c r="K117" s="25" t="s"/>
       <c r="L117" s="7" t="s"/>
     </row>
     <row r="118" spans="1:12">
@@ -2865,9 +2950,9 @@
       <c r="F118" s="7" t="s"/>
       <c r="G118" s="7" t="s"/>
       <c r="H118" s="4" t="s"/>
-      <c r="I118" s="24" t="s"/>
-      <c r="J118" s="24" t="s"/>
-      <c r="K118" s="24" t="s"/>
+      <c r="I118" s="25" t="s"/>
+      <c r="J118" s="25" t="s"/>
+      <c r="K118" s="25" t="s"/>
       <c r="L118" s="7" t="s"/>
     </row>
     <row r="119" spans="1:12">
@@ -2879,9 +2964,9 @@
       <c r="F119" s="7" t="s"/>
       <c r="G119" s="7" t="s"/>
       <c r="H119" s="4" t="s"/>
-      <c r="I119" s="24" t="s"/>
-      <c r="J119" s="24" t="s"/>
-      <c r="K119" s="24" t="s"/>
+      <c r="I119" s="25" t="s"/>
+      <c r="J119" s="25" t="s"/>
+      <c r="K119" s="25" t="s"/>
       <c r="L119" s="7" t="s"/>
     </row>
     <row r="120" spans="1:12">
@@ -2893,9 +2978,9 @@
       <c r="F120" s="7" t="s"/>
       <c r="G120" s="7" t="s"/>
       <c r="H120" s="4" t="s"/>
-      <c r="I120" s="24" t="s"/>
-      <c r="J120" s="24" t="s"/>
-      <c r="K120" s="24" t="s"/>
+      <c r="I120" s="25" t="s"/>
+      <c r="J120" s="25" t="s"/>
+      <c r="K120" s="25" t="s"/>
       <c r="L120" s="7" t="s"/>
     </row>
     <row r="121" spans="1:12">
@@ -2907,9 +2992,9 @@
       <c r="F121" s="7" t="s"/>
       <c r="G121" s="7" t="s"/>
       <c r="H121" s="4" t="s"/>
-      <c r="I121" s="24" t="s"/>
-      <c r="J121" s="24" t="s"/>
-      <c r="K121" s="24" t="s"/>
+      <c r="I121" s="25" t="s"/>
+      <c r="J121" s="25" t="s"/>
+      <c r="K121" s="25" t="s"/>
       <c r="L121" s="7" t="s"/>
     </row>
     <row r="122" spans="1:12">
@@ -2921,9 +3006,9 @@
       <c r="F122" s="7" t="s"/>
       <c r="G122" s="7" t="s"/>
       <c r="H122" s="4" t="s"/>
-      <c r="I122" s="24" t="s"/>
-      <c r="J122" s="24" t="s"/>
-      <c r="K122" s="24" t="s"/>
+      <c r="I122" s="25" t="s"/>
+      <c r="J122" s="25" t="s"/>
+      <c r="K122" s="25" t="s"/>
       <c r="L122" s="7" t="s"/>
     </row>
     <row r="123" spans="1:12">
@@ -2935,9 +3020,9 @@
       <c r="F123" s="7" t="s"/>
       <c r="G123" s="7" t="s"/>
       <c r="H123" s="4" t="s"/>
-      <c r="I123" s="24" t="s"/>
-      <c r="J123" s="24" t="s"/>
-      <c r="K123" s="24" t="s"/>
+      <c r="I123" s="25" t="s"/>
+      <c r="J123" s="25" t="s"/>
+      <c r="K123" s="25" t="s"/>
       <c r="L123" s="7" t="s"/>
     </row>
     <row r="124" spans="1:12">
@@ -2949,9 +3034,9 @@
       <c r="F124" s="7" t="s"/>
       <c r="G124" s="7" t="s"/>
       <c r="H124" s="4" t="s"/>
-      <c r="I124" s="24" t="s"/>
-      <c r="J124" s="24" t="s"/>
-      <c r="K124" s="24" t="s"/>
+      <c r="I124" s="25" t="s"/>
+      <c r="J124" s="25" t="s"/>
+      <c r="K124" s="25" t="s"/>
       <c r="L124" s="7" t="s"/>
     </row>
     <row r="125" spans="1:12">
@@ -2963,9 +3048,9 @@
       <c r="F125" s="7" t="s"/>
       <c r="G125" s="7" t="s"/>
       <c r="H125" s="4" t="s"/>
-      <c r="I125" s="24" t="s"/>
-      <c r="J125" s="24" t="s"/>
-      <c r="K125" s="24" t="s"/>
+      <c r="I125" s="25" t="s"/>
+      <c r="J125" s="25" t="s"/>
+      <c r="K125" s="25" t="s"/>
       <c r="L125" s="7" t="s"/>
     </row>
     <row r="126" spans="1:12">
@@ -2977,9 +3062,9 @@
       <c r="F126" s="7" t="s"/>
       <c r="G126" s="7" t="s"/>
       <c r="H126" s="4" t="s"/>
-      <c r="I126" s="24" t="s"/>
-      <c r="J126" s="24" t="s"/>
-      <c r="K126" s="24" t="s"/>
+      <c r="I126" s="25" t="s"/>
+      <c r="J126" s="25" t="s"/>
+      <c r="K126" s="25" t="s"/>
       <c r="L126" s="7" t="s"/>
     </row>
     <row r="127" spans="1:12">
@@ -2991,9 +3076,9 @@
       <c r="F127" s="7" t="s"/>
       <c r="G127" s="7" t="s"/>
       <c r="H127" s="4" t="s"/>
-      <c r="I127" s="24" t="s"/>
-      <c r="J127" s="24" t="s"/>
-      <c r="K127" s="24" t="s"/>
+      <c r="I127" s="25" t="s"/>
+      <c r="J127" s="25" t="s"/>
+      <c r="K127" s="25" t="s"/>
       <c r="L127" s="7" t="s"/>
     </row>
     <row r="128" spans="1:12">
@@ -3005,9 +3090,9 @@
       <c r="F128" s="7" t="s"/>
       <c r="G128" s="7" t="s"/>
       <c r="H128" s="4" t="s"/>
-      <c r="I128" s="24" t="s"/>
-      <c r="J128" s="24" t="s"/>
-      <c r="K128" s="24" t="s"/>
+      <c r="I128" s="25" t="s"/>
+      <c r="J128" s="25" t="s"/>
+      <c r="K128" s="25" t="s"/>
       <c r="L128" s="7" t="s"/>
     </row>
     <row r="129" spans="1:12">
@@ -3019,9 +3104,9 @@
       <c r="F129" s="7" t="s"/>
       <c r="G129" s="7" t="s"/>
       <c r="H129" s="4" t="s"/>
-      <c r="I129" s="24" t="s"/>
-      <c r="J129" s="24" t="s"/>
-      <c r="K129" s="24" t="s"/>
+      <c r="I129" s="25" t="s"/>
+      <c r="J129" s="25" t="s"/>
+      <c r="K129" s="25" t="s"/>
       <c r="L129" s="7" t="s"/>
     </row>
     <row r="130" spans="1:12">
@@ -3033,9 +3118,9 @@
       <c r="F130" s="7" t="s"/>
       <c r="G130" s="7" t="s"/>
       <c r="H130" s="4" t="s"/>
-      <c r="I130" s="24" t="s"/>
-      <c r="J130" s="24" t="s"/>
-      <c r="K130" s="24" t="s"/>
+      <c r="I130" s="25" t="s"/>
+      <c r="J130" s="25" t="s"/>
+      <c r="K130" s="25" t="s"/>
       <c r="L130" s="7" t="s"/>
     </row>
     <row r="131" spans="1:12">
@@ -3047,9 +3132,9 @@
       <c r="F131" s="7" t="s"/>
       <c r="G131" s="7" t="s"/>
       <c r="H131" s="4" t="s"/>
-      <c r="I131" s="24" t="s"/>
-      <c r="J131" s="24" t="s"/>
-      <c r="K131" s="24" t="s"/>
+      <c r="I131" s="25" t="s"/>
+      <c r="J131" s="25" t="s"/>
+      <c r="K131" s="25" t="s"/>
       <c r="L131" s="7" t="s"/>
     </row>
     <row r="132" spans="1:12">
@@ -3061,9 +3146,9 @@
       <c r="F132" s="7" t="s"/>
       <c r="G132" s="7" t="s"/>
       <c r="H132" s="4" t="s"/>
-      <c r="I132" s="24" t="s"/>
-      <c r="J132" s="24" t="s"/>
-      <c r="K132" s="24" t="s"/>
+      <c r="I132" s="25" t="s"/>
+      <c r="J132" s="25" t="s"/>
+      <c r="K132" s="25" t="s"/>
       <c r="L132" s="7" t="s"/>
     </row>
     <row r="133" spans="1:12">
@@ -3075,9 +3160,9 @@
       <c r="F133" s="7" t="s"/>
       <c r="G133" s="7" t="s"/>
       <c r="H133" s="4" t="s"/>
-      <c r="I133" s="24" t="s"/>
-      <c r="J133" s="24" t="s"/>
-      <c r="K133" s="24" t="s"/>
+      <c r="I133" s="25" t="s"/>
+      <c r="J133" s="25" t="s"/>
+      <c r="K133" s="25" t="s"/>
       <c r="L133" s="7" t="s"/>
     </row>
     <row r="134" spans="1:12">
@@ -3089,9 +3174,9 @@
       <c r="F134" s="7" t="s"/>
       <c r="G134" s="7" t="s"/>
       <c r="H134" s="4" t="s"/>
-      <c r="I134" s="24" t="s"/>
-      <c r="J134" s="24" t="s"/>
-      <c r="K134" s="24" t="s"/>
+      <c r="I134" s="25" t="s"/>
+      <c r="J134" s="25" t="s"/>
+      <c r="K134" s="25" t="s"/>
       <c r="L134" s="7" t="s"/>
     </row>
     <row r="135" spans="1:12">
@@ -3103,9 +3188,9 @@
       <c r="F135" s="7" t="s"/>
       <c r="G135" s="7" t="s"/>
       <c r="H135" s="4" t="s"/>
-      <c r="I135" s="24" t="s"/>
-      <c r="J135" s="24" t="s"/>
-      <c r="K135" s="24" t="s"/>
+      <c r="I135" s="25" t="s"/>
+      <c r="J135" s="25" t="s"/>
+      <c r="K135" s="25" t="s"/>
       <c r="L135" s="7" t="s"/>
     </row>
     <row r="136" spans="1:12">
@@ -3117,9 +3202,9 @@
       <c r="F136" s="7" t="s"/>
       <c r="G136" s="7" t="s"/>
       <c r="H136" s="4" t="s"/>
-      <c r="I136" s="24" t="s"/>
-      <c r="J136" s="24" t="s"/>
-      <c r="K136" s="24" t="s"/>
+      <c r="I136" s="25" t="s"/>
+      <c r="J136" s="25" t="s"/>
+      <c r="K136" s="25" t="s"/>
       <c r="L136" s="7" t="s"/>
     </row>
     <row r="137" spans="1:12">
@@ -3131,9 +3216,9 @@
       <c r="F137" s="7" t="s"/>
       <c r="G137" s="7" t="s"/>
       <c r="H137" s="4" t="s"/>
-      <c r="I137" s="24" t="s"/>
-      <c r="J137" s="24" t="s"/>
-      <c r="K137" s="24" t="s"/>
+      <c r="I137" s="25" t="s"/>
+      <c r="J137" s="25" t="s"/>
+      <c r="K137" s="25" t="s"/>
       <c r="L137" s="7" t="s"/>
     </row>
     <row r="138" spans="1:12">
@@ -3145,9 +3230,9 @@
       <c r="F138" s="7" t="s"/>
       <c r="G138" s="7" t="s"/>
       <c r="H138" s="4" t="s"/>
-      <c r="I138" s="24" t="s"/>
-      <c r="J138" s="24" t="s"/>
-      <c r="K138" s="24" t="s"/>
+      <c r="I138" s="25" t="s"/>
+      <c r="J138" s="25" t="s"/>
+      <c r="K138" s="25" t="s"/>
       <c r="L138" s="7" t="s"/>
     </row>
     <row r="139" spans="1:12">
@@ -3159,9 +3244,9 @@
       <c r="F139" s="7" t="s"/>
       <c r="G139" s="7" t="s"/>
       <c r="H139" s="4" t="s"/>
-      <c r="I139" s="24" t="s"/>
-      <c r="J139" s="24" t="s"/>
-      <c r="K139" s="24" t="s"/>
+      <c r="I139" s="25" t="s"/>
+      <c r="J139" s="25" t="s"/>
+      <c r="K139" s="25" t="s"/>
       <c r="L139" s="7" t="s"/>
     </row>
     <row r="140" spans="1:12">
@@ -3173,9 +3258,9 @@
       <c r="F140" s="7" t="s"/>
       <c r="G140" s="7" t="s"/>
       <c r="H140" s="4" t="s"/>
-      <c r="I140" s="24" t="s"/>
-      <c r="J140" s="24" t="s"/>
-      <c r="K140" s="24" t="s"/>
+      <c r="I140" s="25" t="s"/>
+      <c r="J140" s="25" t="s"/>
+      <c r="K140" s="25" t="s"/>
       <c r="L140" s="7" t="s"/>
     </row>
     <row r="141" spans="1:12">
@@ -3187,9 +3272,9 @@
       <c r="F141" s="7" t="s"/>
       <c r="G141" s="7" t="s"/>
       <c r="H141" s="4" t="s"/>
-      <c r="I141" s="24" t="s"/>
-      <c r="J141" s="24" t="s"/>
-      <c r="K141" s="24" t="s"/>
+      <c r="I141" s="25" t="s"/>
+      <c r="J141" s="25" t="s"/>
+      <c r="K141" s="25" t="s"/>
       <c r="L141" s="7" t="s"/>
     </row>
     <row r="142" spans="1:12">
@@ -3201,9 +3286,9 @@
       <c r="F142" s="7" t="s"/>
       <c r="G142" s="7" t="s"/>
       <c r="H142" s="4" t="s"/>
-      <c r="I142" s="24" t="s"/>
-      <c r="J142" s="24" t="s"/>
-      <c r="K142" s="24" t="s"/>
+      <c r="I142" s="25" t="s"/>
+      <c r="J142" s="25" t="s"/>
+      <c r="K142" s="25" t="s"/>
       <c r="L142" s="7" t="s"/>
     </row>
     <row r="143" spans="1:12">
@@ -3215,9 +3300,9 @@
       <c r="F143" s="7" t="s"/>
       <c r="G143" s="7" t="s"/>
       <c r="H143" s="4" t="s"/>
-      <c r="I143" s="24" t="s"/>
-      <c r="J143" s="24" t="s"/>
-      <c r="K143" s="24" t="s"/>
+      <c r="I143" s="25" t="s"/>
+      <c r="J143" s="25" t="s"/>
+      <c r="K143" s="25" t="s"/>
       <c r="L143" s="7" t="s"/>
     </row>
     <row r="144" spans="1:12">
@@ -3229,9 +3314,9 @@
       <c r="F144" s="7" t="s"/>
       <c r="G144" s="7" t="s"/>
       <c r="H144" s="4" t="s"/>
-      <c r="I144" s="24" t="s"/>
-      <c r="J144" s="24" t="s"/>
-      <c r="K144" s="24" t="s"/>
+      <c r="I144" s="25" t="s"/>
+      <c r="J144" s="25" t="s"/>
+      <c r="K144" s="25" t="s"/>
       <c r="L144" s="7" t="s"/>
     </row>
     <row r="145" spans="1:12">
@@ -3243,9 +3328,9 @@
       <c r="F145" s="7" t="s"/>
       <c r="G145" s="7" t="s"/>
       <c r="H145" s="4" t="s"/>
-      <c r="I145" s="24" t="s"/>
-      <c r="J145" s="24" t="s"/>
-      <c r="K145" s="24" t="s"/>
+      <c r="I145" s="25" t="s"/>
+      <c r="J145" s="25" t="s"/>
+      <c r="K145" s="25" t="s"/>
       <c r="L145" s="7" t="s"/>
     </row>
     <row r="146" spans="1:12">
@@ -3257,9 +3342,9 @@
       <c r="F146" s="7" t="s"/>
       <c r="G146" s="7" t="s"/>
       <c r="H146" s="4" t="s"/>
-      <c r="I146" s="24" t="s"/>
-      <c r="J146" s="24" t="s"/>
-      <c r="K146" s="24" t="s"/>
+      <c r="I146" s="25" t="s"/>
+      <c r="J146" s="25" t="s"/>
+      <c r="K146" s="25" t="s"/>
       <c r="L146" s="7" t="s"/>
     </row>
     <row r="147" spans="1:12">
@@ -3271,9 +3356,9 @@
       <c r="F147" s="7" t="s"/>
       <c r="G147" s="7" t="s"/>
       <c r="H147" s="4" t="s"/>
-      <c r="I147" s="24" t="s"/>
-      <c r="J147" s="24" t="s"/>
-      <c r="K147" s="24" t="s"/>
+      <c r="I147" s="25" t="s"/>
+      <c r="J147" s="25" t="s"/>
+      <c r="K147" s="25" t="s"/>
       <c r="L147" s="7" t="s"/>
     </row>
     <row r="148" spans="1:12">
@@ -3285,9 +3370,9 @@
       <c r="F148" s="7" t="s"/>
       <c r="G148" s="7" t="s"/>
       <c r="H148" s="4" t="s"/>
-      <c r="I148" s="24" t="s"/>
-      <c r="J148" s="24" t="s"/>
-      <c r="K148" s="24" t="s"/>
+      <c r="I148" s="25" t="s"/>
+      <c r="J148" s="25" t="s"/>
+      <c r="K148" s="25" t="s"/>
       <c r="L148" s="7" t="s"/>
     </row>
     <row r="149" spans="1:12">
@@ -3299,9 +3384,9 @@
       <c r="F149" s="7" t="s"/>
       <c r="G149" s="7" t="s"/>
       <c r="H149" s="4" t="s"/>
-      <c r="I149" s="24" t="s"/>
-      <c r="J149" s="24" t="s"/>
-      <c r="K149" s="24" t="s"/>
+      <c r="I149" s="25" t="s"/>
+      <c r="J149" s="25" t="s"/>
+      <c r="K149" s="25" t="s"/>
       <c r="L149" s="7" t="s"/>
     </row>
     <row r="150" spans="1:12">
@@ -3313,9 +3398,9 @@
       <c r="F150" s="7" t="s"/>
       <c r="G150" s="7" t="s"/>
       <c r="H150" s="4" t="s"/>
-      <c r="I150" s="24" t="s"/>
-      <c r="J150" s="24" t="s"/>
-      <c r="K150" s="24" t="s"/>
+      <c r="I150" s="25" t="s"/>
+      <c r="J150" s="25" t="s"/>
+      <c r="K150" s="25" t="s"/>
       <c r="L150" s="7" t="s"/>
     </row>
     <row r="151" spans="1:12">
@@ -3327,9 +3412,9 @@
       <c r="F151" s="7" t="s"/>
       <c r="G151" s="7" t="s"/>
       <c r="H151" s="4" t="s"/>
-      <c r="I151" s="24" t="s"/>
-      <c r="J151" s="24" t="s"/>
-      <c r="K151" s="24" t="s"/>
+      <c r="I151" s="25" t="s"/>
+      <c r="J151" s="25" t="s"/>
+      <c r="K151" s="25" t="s"/>
       <c r="L151" s="7" t="s"/>
     </row>
     <row r="152" spans="1:12">
@@ -3341,9 +3426,9 @@
       <c r="F152" s="7" t="s"/>
       <c r="G152" s="7" t="s"/>
       <c r="H152" s="4" t="s"/>
-      <c r="I152" s="24" t="s"/>
-      <c r="J152" s="24" t="s"/>
-      <c r="K152" s="24" t="s"/>
+      <c r="I152" s="25" t="s"/>
+      <c r="J152" s="25" t="s"/>
+      <c r="K152" s="25" t="s"/>
       <c r="L152" s="7" t="s"/>
     </row>
     <row r="153" spans="1:12">
@@ -3355,9 +3440,9 @@
       <c r="F153" s="7" t="s"/>
       <c r="G153" s="7" t="s"/>
       <c r="H153" s="4" t="s"/>
-      <c r="I153" s="24" t="s"/>
-      <c r="J153" s="24" t="s"/>
-      <c r="K153" s="24" t="s"/>
+      <c r="I153" s="25" t="s"/>
+      <c r="J153" s="25" t="s"/>
+      <c r="K153" s="25" t="s"/>
       <c r="L153" s="7" t="s"/>
     </row>
     <row r="154" spans="1:12">
@@ -3369,9 +3454,9 @@
       <c r="F154" s="7" t="s"/>
       <c r="G154" s="7" t="s"/>
       <c r="H154" s="4" t="s"/>
-      <c r="I154" s="24" t="s"/>
-      <c r="J154" s="24" t="s"/>
-      <c r="K154" s="24" t="s"/>
+      <c r="I154" s="25" t="s"/>
+      <c r="J154" s="25" t="s"/>
+      <c r="K154" s="25" t="s"/>
       <c r="L154" s="7" t="s"/>
     </row>
     <row r="155" spans="1:12">
@@ -3383,9 +3468,9 @@
       <c r="F155" s="7" t="s"/>
       <c r="G155" s="7" t="s"/>
       <c r="H155" s="4" t="s"/>
-      <c r="I155" s="24" t="s"/>
-      <c r="J155" s="24" t="s"/>
-      <c r="K155" s="24" t="s"/>
+      <c r="I155" s="25" t="s"/>
+      <c r="J155" s="25" t="s"/>
+      <c r="K155" s="25" t="s"/>
       <c r="L155" s="7" t="s"/>
     </row>
     <row r="156" spans="1:12">
@@ -3397,9 +3482,9 @@
       <c r="F156" s="7" t="s"/>
       <c r="G156" s="7" t="s"/>
       <c r="H156" s="4" t="s"/>
-      <c r="I156" s="24" t="s"/>
-      <c r="J156" s="24" t="s"/>
-      <c r="K156" s="24" t="s"/>
+      <c r="I156" s="25" t="s"/>
+      <c r="J156" s="25" t="s"/>
+      <c r="K156" s="25" t="s"/>
       <c r="L156" s="7" t="s"/>
     </row>
     <row r="157" spans="1:12">
@@ -3411,9 +3496,9 @@
       <c r="F157" s="7" t="s"/>
       <c r="G157" s="7" t="s"/>
       <c r="H157" s="4" t="s"/>
-      <c r="I157" s="24" t="s"/>
-      <c r="J157" s="24" t="s"/>
-      <c r="K157" s="24" t="s"/>
+      <c r="I157" s="25" t="s"/>
+      <c r="J157" s="25" t="s"/>
+      <c r="K157" s="25" t="s"/>
       <c r="L157" s="7" t="s"/>
     </row>
     <row r="158" spans="1:12">
@@ -3425,9 +3510,9 @@
       <c r="F158" s="7" t="s"/>
       <c r="G158" s="7" t="s"/>
       <c r="H158" s="4" t="s"/>
-      <c r="I158" s="24" t="s"/>
-      <c r="J158" s="24" t="s"/>
-      <c r="K158" s="24" t="s"/>
+      <c r="I158" s="25" t="s"/>
+      <c r="J158" s="25" t="s"/>
+      <c r="K158" s="25" t="s"/>
       <c r="L158" s="7" t="s"/>
     </row>
     <row r="159" spans="1:12">
@@ -3439,9 +3524,9 @@
       <c r="F159" s="7" t="s"/>
       <c r="G159" s="7" t="s"/>
       <c r="H159" s="4" t="s"/>
-      <c r="I159" s="24" t="s"/>
-      <c r="J159" s="24" t="s"/>
-      <c r="K159" s="24" t="s"/>
+      <c r="I159" s="25" t="s"/>
+      <c r="J159" s="25" t="s"/>
+      <c r="K159" s="25" t="s"/>
       <c r="L159" s="7" t="s"/>
     </row>
     <row r="160" spans="1:12">
@@ -3453,9 +3538,9 @@
       <c r="F160" s="7" t="s"/>
       <c r="G160" s="7" t="s"/>
       <c r="H160" s="4" t="s"/>
-      <c r="I160" s="24" t="s"/>
-      <c r="J160" s="24" t="s"/>
-      <c r="K160" s="24" t="s"/>
+      <c r="I160" s="25" t="s"/>
+      <c r="J160" s="25" t="s"/>
+      <c r="K160" s="25" t="s"/>
       <c r="L160" s="7" t="s"/>
     </row>
     <row r="161" spans="1:12">
@@ -3467,9 +3552,9 @@
       <c r="F161" s="7" t="s"/>
       <c r="G161" s="7" t="s"/>
       <c r="H161" s="4" t="s"/>
-      <c r="I161" s="24" t="s"/>
-      <c r="J161" s="24" t="s"/>
-      <c r="K161" s="24" t="s"/>
+      <c r="I161" s="25" t="s"/>
+      <c r="J161" s="25" t="s"/>
+      <c r="K161" s="25" t="s"/>
       <c r="L161" s="7" t="s"/>
     </row>
     <row r="162" spans="1:12">
@@ -3481,9 +3566,9 @@
       <c r="F162" s="7" t="s"/>
       <c r="G162" s="7" t="s"/>
       <c r="H162" s="4" t="s"/>
-      <c r="I162" s="24" t="s"/>
-      <c r="J162" s="24" t="s"/>
-      <c r="K162" s="24" t="s"/>
+      <c r="I162" s="25" t="s"/>
+      <c r="J162" s="25" t="s"/>
+      <c r="K162" s="25" t="s"/>
       <c r="L162" s="7" t="s"/>
     </row>
     <row r="163" spans="1:12">
@@ -3495,9 +3580,9 @@
       <c r="F163" s="7" t="s"/>
       <c r="G163" s="7" t="s"/>
       <c r="H163" s="4" t="s"/>
-      <c r="I163" s="24" t="s"/>
-      <c r="J163" s="24" t="s"/>
-      <c r="K163" s="24" t="s"/>
+      <c r="I163" s="25" t="s"/>
+      <c r="J163" s="25" t="s"/>
+      <c r="K163" s="25" t="s"/>
       <c r="L163" s="7" t="s"/>
     </row>
     <row r="164" spans="1:12">
@@ -3509,9 +3594,9 @@
       <c r="F164" s="7" t="s"/>
       <c r="G164" s="7" t="s"/>
       <c r="H164" s="4" t="s"/>
-      <c r="I164" s="24" t="s"/>
-      <c r="J164" s="24" t="s"/>
-      <c r="K164" s="24" t="s"/>
+      <c r="I164" s="25" t="s"/>
+      <c r="J164" s="25" t="s"/>
+      <c r="K164" s="25" t="s"/>
       <c r="L164" s="7" t="s"/>
     </row>
     <row r="165" spans="1:12">
@@ -3523,9 +3608,9 @@
       <c r="F165" s="7" t="s"/>
       <c r="G165" s="7" t="s"/>
       <c r="H165" s="4" t="s"/>
-      <c r="I165" s="24" t="s"/>
-      <c r="J165" s="24" t="s"/>
-      <c r="K165" s="24" t="s"/>
+      <c r="I165" s="25" t="s"/>
+      <c r="J165" s="25" t="s"/>
+      <c r="K165" s="25" t="s"/>
       <c r="L165" s="7" t="s"/>
     </row>
     <row r="166" spans="1:12">
@@ -3537,9 +3622,9 @@
       <c r="F166" s="7" t="s"/>
       <c r="G166" s="7" t="s"/>
       <c r="H166" s="4" t="s"/>
-      <c r="I166" s="24" t="s"/>
-      <c r="J166" s="24" t="s"/>
-      <c r="K166" s="24" t="s"/>
+      <c r="I166" s="25" t="s"/>
+      <c r="J166" s="25" t="s"/>
+      <c r="K166" s="25" t="s"/>
       <c r="L166" s="7" t="s"/>
     </row>
     <row r="167" spans="1:12">
@@ -3551,9 +3636,9 @@
       <c r="F167" s="7" t="s"/>
       <c r="G167" s="7" t="s"/>
       <c r="H167" s="4" t="s"/>
-      <c r="I167" s="24" t="s"/>
-      <c r="J167" s="24" t="s"/>
-      <c r="K167" s="24" t="s"/>
+      <c r="I167" s="25" t="s"/>
+      <c r="J167" s="25" t="s"/>
+      <c r="K167" s="25" t="s"/>
       <c r="L167" s="7" t="s"/>
     </row>
     <row r="168" spans="1:12">
@@ -3565,9 +3650,9 @@
       <c r="F168" s="7" t="s"/>
       <c r="G168" s="7" t="s"/>
       <c r="H168" s="4" t="s"/>
-      <c r="I168" s="24" t="s"/>
-      <c r="J168" s="24" t="s"/>
-      <c r="K168" s="24" t="s"/>
+      <c r="I168" s="25" t="s"/>
+      <c r="J168" s="25" t="s"/>
+      <c r="K168" s="25" t="s"/>
       <c r="L168" s="7" t="s"/>
     </row>
     <row r="169" spans="1:12">
@@ -3579,9 +3664,9 @@
       <c r="F169" s="7" t="s"/>
       <c r="G169" s="7" t="s"/>
       <c r="H169" s="4" t="s"/>
-      <c r="I169" s="24" t="s"/>
-      <c r="J169" s="24" t="s"/>
-      <c r="K169" s="24" t="s"/>
+      <c r="I169" s="25" t="s"/>
+      <c r="J169" s="25" t="s"/>
+      <c r="K169" s="25" t="s"/>
       <c r="L169" s="7" t="s"/>
     </row>
     <row r="170" spans="1:12">
@@ -3593,9 +3678,9 @@
       <c r="F170" s="7" t="s"/>
       <c r="G170" s="7" t="s"/>
       <c r="H170" s="4" t="s"/>
-      <c r="I170" s="24" t="s"/>
-      <c r="J170" s="24" t="s"/>
-      <c r="K170" s="24" t="s"/>
+      <c r="I170" s="25" t="s"/>
+      <c r="J170" s="25" t="s"/>
+      <c r="K170" s="25" t="s"/>
       <c r="L170" s="7" t="s"/>
     </row>
     <row r="171" spans="1:12">
@@ -3607,9 +3692,9 @@
       <c r="F171" s="7" t="s"/>
       <c r="G171" s="7" t="s"/>
       <c r="H171" s="4" t="s"/>
-      <c r="I171" s="24" t="s"/>
-      <c r="J171" s="24" t="s"/>
-      <c r="K171" s="24" t="s"/>
+      <c r="I171" s="25" t="s"/>
+      <c r="J171" s="25" t="s"/>
+      <c r="K171" s="25" t="s"/>
       <c r="L171" s="7" t="s"/>
     </row>
     <row r="172" spans="1:12">
@@ -3621,9 +3706,9 @@
       <c r="F172" s="7" t="s"/>
       <c r="G172" s="7" t="s"/>
       <c r="H172" s="4" t="s"/>
-      <c r="I172" s="24" t="s"/>
-      <c r="J172" s="24" t="s"/>
-      <c r="K172" s="24" t="s"/>
+      <c r="I172" s="25" t="s"/>
+      <c r="J172" s="25" t="s"/>
+      <c r="K172" s="25" t="s"/>
       <c r="L172" s="7" t="s"/>
     </row>
     <row r="173" spans="1:12">
@@ -3635,9 +3720,9 @@
       <c r="F173" s="7" t="s"/>
       <c r="G173" s="7" t="s"/>
       <c r="H173" s="4" t="s"/>
-      <c r="I173" s="24" t="s"/>
-      <c r="J173" s="24" t="s"/>
-      <c r="K173" s="24" t="s"/>
+      <c r="I173" s="25" t="s"/>
+      <c r="J173" s="25" t="s"/>
+      <c r="K173" s="25" t="s"/>
       <c r="L173" s="7" t="s"/>
     </row>
     <row r="174" spans="1:12">
@@ -3649,9 +3734,9 @@
       <c r="F174" s="7" t="s"/>
       <c r="G174" s="7" t="s"/>
       <c r="H174" s="4" t="s"/>
-      <c r="I174" s="24" t="s"/>
-      <c r="J174" s="24" t="s"/>
-      <c r="K174" s="24" t="s"/>
+      <c r="I174" s="25" t="s"/>
+      <c r="J174" s="25" t="s"/>
+      <c r="K174" s="25" t="s"/>
       <c r="L174" s="7" t="s"/>
     </row>
     <row r="175" spans="1:12">
@@ -3663,9 +3748,9 @@
       <c r="F175" s="7" t="s"/>
       <c r="G175" s="7" t="s"/>
       <c r="H175" s="4" t="s"/>
-      <c r="I175" s="24" t="s"/>
-      <c r="J175" s="24" t="s"/>
-      <c r="K175" s="24" t="s"/>
+      <c r="I175" s="25" t="s"/>
+      <c r="J175" s="25" t="s"/>
+      <c r="K175" s="25" t="s"/>
       <c r="L175" s="7" t="s"/>
     </row>
     <row r="176" spans="1:12">
@@ -3677,9 +3762,9 @@
       <c r="F176" s="7" t="s"/>
       <c r="G176" s="7" t="s"/>
       <c r="H176" s="4" t="s"/>
-      <c r="I176" s="24" t="s"/>
-      <c r="J176" s="24" t="s"/>
-      <c r="K176" s="24" t="s"/>
+      <c r="I176" s="25" t="s"/>
+      <c r="J176" s="25" t="s"/>
+      <c r="K176" s="25" t="s"/>
       <c r="L176" s="7" t="s"/>
     </row>
     <row r="177" spans="1:12">
@@ -3691,9 +3776,9 @@
       <c r="F177" s="7" t="s"/>
       <c r="G177" s="7" t="s"/>
       <c r="H177" s="4" t="s"/>
-      <c r="I177" s="24" t="s"/>
-      <c r="J177" s="24" t="s"/>
-      <c r="K177" s="24" t="s"/>
+      <c r="I177" s="25" t="s"/>
+      <c r="J177" s="25" t="s"/>
+      <c r="K177" s="25" t="s"/>
       <c r="L177" s="7" t="s"/>
     </row>
     <row r="178" spans="1:12">
@@ -3705,9 +3790,9 @@
       <c r="F178" s="7" t="s"/>
       <c r="G178" s="7" t="s"/>
       <c r="H178" s="4" t="s"/>
-      <c r="I178" s="24" t="s"/>
-      <c r="J178" s="24" t="s"/>
-      <c r="K178" s="24" t="s"/>
+      <c r="I178" s="25" t="s"/>
+      <c r="J178" s="25" t="s"/>
+      <c r="K178" s="25" t="s"/>
       <c r="L178" s="7" t="s"/>
     </row>
     <row r="179" spans="1:12">
@@ -3719,9 +3804,9 @@
       <c r="F179" s="7" t="s"/>
       <c r="G179" s="7" t="s"/>
       <c r="H179" s="4" t="s"/>
-      <c r="I179" s="24" t="s"/>
-      <c r="J179" s="24" t="s"/>
-      <c r="K179" s="24" t="s"/>
+      <c r="I179" s="25" t="s"/>
+      <c r="J179" s="25" t="s"/>
+      <c r="K179" s="25" t="s"/>
       <c r="L179" s="7" t="s"/>
     </row>
     <row r="180" spans="1:12">
@@ -3733,9 +3818,9 @@
       <c r="F180" s="7" t="s"/>
       <c r="G180" s="7" t="s"/>
       <c r="H180" s="4" t="s"/>
-      <c r="I180" s="24" t="s"/>
-      <c r="J180" s="24" t="s"/>
-      <c r="K180" s="24" t="s"/>
+      <c r="I180" s="25" t="s"/>
+      <c r="J180" s="25" t="s"/>
+      <c r="K180" s="25" t="s"/>
       <c r="L180" s="7" t="s"/>
     </row>
     <row r="181" spans="1:12">
@@ -3747,9 +3832,9 @@
       <c r="F181" s="7" t="s"/>
       <c r="G181" s="7" t="s"/>
       <c r="H181" s="4" t="s"/>
-      <c r="I181" s="24" t="s"/>
-      <c r="J181" s="24" t="s"/>
-      <c r="K181" s="24" t="s"/>
+      <c r="I181" s="25" t="s"/>
+      <c r="J181" s="25" t="s"/>
+      <c r="K181" s="25" t="s"/>
       <c r="L181" s="7" t="s"/>
     </row>
     <row r="182" spans="1:12">
@@ -3761,9 +3846,9 @@
       <c r="F182" s="7" t="s"/>
       <c r="G182" s="7" t="s"/>
       <c r="H182" s="4" t="s"/>
-      <c r="I182" s="24" t="s"/>
-      <c r="J182" s="24" t="s"/>
-      <c r="K182" s="24" t="s"/>
+      <c r="I182" s="25" t="s"/>
+      <c r="J182" s="25" t="s"/>
+      <c r="K182" s="25" t="s"/>
       <c r="L182" s="7" t="s"/>
     </row>
     <row r="183" spans="1:12">
@@ -3775,9 +3860,9 @@
       <c r="F183" s="7" t="s"/>
       <c r="G183" s="7" t="s"/>
       <c r="H183" s="4" t="s"/>
-      <c r="I183" s="24" t="s"/>
-      <c r="J183" s="24" t="s"/>
-      <c r="K183" s="24" t="s"/>
+      <c r="I183" s="25" t="s"/>
+      <c r="J183" s="25" t="s"/>
+      <c r="K183" s="25" t="s"/>
       <c r="L183" s="7" t="s"/>
     </row>
     <row r="184" spans="1:12">
@@ -3789,9 +3874,9 @@
       <c r="F184" s="7" t="s"/>
       <c r="G184" s="7" t="s"/>
       <c r="H184" s="4" t="s"/>
-      <c r="I184" s="24" t="s"/>
-      <c r="J184" s="24" t="s"/>
-      <c r="K184" s="24" t="s"/>
+      <c r="I184" s="25" t="s"/>
+      <c r="J184" s="25" t="s"/>
+      <c r="K184" s="25" t="s"/>
       <c r="L184" s="7" t="s"/>
     </row>
     <row r="185" spans="1:12">
@@ -3803,9 +3888,9 @@
       <c r="F185" s="7" t="s"/>
       <c r="G185" s="7" t="s"/>
       <c r="H185" s="4" t="s"/>
-      <c r="I185" s="24" t="s"/>
-      <c r="J185" s="24" t="s"/>
-      <c r="K185" s="24" t="s"/>
+      <c r="I185" s="25" t="s"/>
+      <c r="J185" s="25" t="s"/>
+      <c r="K185" s="25" t="s"/>
       <c r="L185" s="7" t="s"/>
     </row>
     <row r="186" spans="1:12">
@@ -3817,9 +3902,9 @@
       <c r="F186" s="7" t="s"/>
       <c r="G186" s="7" t="s"/>
       <c r="H186" s="4" t="s"/>
-      <c r="I186" s="24" t="s"/>
-      <c r="J186" s="24" t="s"/>
-      <c r="K186" s="24" t="s"/>
+      <c r="I186" s="25" t="s"/>
+      <c r="J186" s="25" t="s"/>
+      <c r="K186" s="25" t="s"/>
       <c r="L186" s="7" t="s"/>
     </row>
     <row r="187" spans="1:12">
@@ -3831,9 +3916,9 @@
       <c r="F187" s="7" t="s"/>
       <c r="G187" s="7" t="s"/>
       <c r="H187" s="4" t="s"/>
-      <c r="I187" s="24" t="s"/>
-      <c r="J187" s="24" t="s"/>
-      <c r="K187" s="24" t="s"/>
+      <c r="I187" s="25" t="s"/>
+      <c r="J187" s="25" t="s"/>
+      <c r="K187" s="25" t="s"/>
       <c r="L187" s="7" t="s"/>
     </row>
     <row r="188" spans="1:12">
@@ -3845,9 +3930,9 @@
       <c r="F188" s="7" t="s"/>
       <c r="G188" s="7" t="s"/>
       <c r="H188" s="4" t="s"/>
-      <c r="I188" s="24" t="s"/>
-      <c r="J188" s="24" t="s"/>
-      <c r="K188" s="24" t="s"/>
+      <c r="I188" s="25" t="s"/>
+      <c r="J188" s="25" t="s"/>
+      <c r="K188" s="25" t="s"/>
       <c r="L188" s="7" t="s"/>
     </row>
     <row r="189" spans="1:12">
@@ -3859,9 +3944,9 @@
       <c r="F189" s="7" t="s"/>
       <c r="G189" s="7" t="s"/>
       <c r="H189" s="4" t="s"/>
-      <c r="I189" s="24" t="s"/>
-      <c r="J189" s="24" t="s"/>
-      <c r="K189" s="24" t="s"/>
+      <c r="I189" s="25" t="s"/>
+      <c r="J189" s="25" t="s"/>
+      <c r="K189" s="25" t="s"/>
       <c r="L189" s="7" t="s"/>
     </row>
     <row r="190" spans="1:12">
@@ -3873,9 +3958,9 @@
       <c r="F190" s="7" t="s"/>
       <c r="G190" s="7" t="s"/>
       <c r="H190" s="4" t="s"/>
-      <c r="I190" s="24" t="s"/>
-      <c r="J190" s="24" t="s"/>
-      <c r="K190" s="24" t="s"/>
+      <c r="I190" s="25" t="s"/>
+      <c r="J190" s="25" t="s"/>
+      <c r="K190" s="25" t="s"/>
       <c r="L190" s="7" t="s"/>
     </row>
     <row r="191" spans="1:12">
@@ -3887,9 +3972,9 @@
       <c r="F191" s="7" t="s"/>
       <c r="G191" s="7" t="s"/>
       <c r="H191" s="4" t="s"/>
-      <c r="I191" s="24" t="s"/>
-      <c r="J191" s="24" t="s"/>
-      <c r="K191" s="24" t="s"/>
+      <c r="I191" s="25" t="s"/>
+      <c r="J191" s="25" t="s"/>
+      <c r="K191" s="25" t="s"/>
       <c r="L191" s="7" t="s"/>
     </row>
     <row r="192" spans="1:12">
@@ -3901,9 +3986,9 @@
       <c r="F192" s="7" t="s"/>
       <c r="G192" s="7" t="s"/>
       <c r="H192" s="4" t="s"/>
-      <c r="I192" s="24" t="s"/>
-      <c r="J192" s="24" t="s"/>
-      <c r="K192" s="24" t="s"/>
+      <c r="I192" s="25" t="s"/>
+      <c r="J192" s="25" t="s"/>
+      <c r="K192" s="25" t="s"/>
       <c r="L192" s="7" t="s"/>
     </row>
     <row r="193" spans="1:12">
@@ -3915,9 +4000,9 @@
       <c r="F193" s="7" t="s"/>
       <c r="G193" s="7" t="s"/>
       <c r="H193" s="4" t="s"/>
-      <c r="I193" s="24" t="s"/>
-      <c r="J193" s="24" t="s"/>
-      <c r="K193" s="24" t="s"/>
+      <c r="I193" s="25" t="s"/>
+      <c r="J193" s="25" t="s"/>
+      <c r="K193" s="25" t="s"/>
       <c r="L193" s="7" t="s"/>
     </row>
     <row r="194" spans="1:12">
@@ -3929,9 +4014,9 @@
       <c r="F194" s="7" t="s"/>
       <c r="G194" s="7" t="s"/>
       <c r="H194" s="4" t="s"/>
-      <c r="I194" s="24" t="s"/>
-      <c r="J194" s="24" t="s"/>
-      <c r="K194" s="24" t="s"/>
+      <c r="I194" s="25" t="s"/>
+      <c r="J194" s="25" t="s"/>
+      <c r="K194" s="25" t="s"/>
       <c r="L194" s="7" t="s"/>
     </row>
     <row r="195" spans="1:12">
@@ -3943,9 +4028,9 @@
       <c r="F195" s="7" t="s"/>
       <c r="G195" s="7" t="s"/>
       <c r="H195" s="4" t="s"/>
-      <c r="I195" s="24" t="s"/>
-      <c r="J195" s="24" t="s"/>
-      <c r="K195" s="24" t="s"/>
+      <c r="I195" s="25" t="s"/>
+      <c r="J195" s="25" t="s"/>
+      <c r="K195" s="25" t="s"/>
       <c r="L195" s="7" t="s"/>
     </row>
     <row r="196" spans="1:12">
@@ -3957,9 +4042,9 @@
       <c r="F196" s="7" t="s"/>
       <c r="G196" s="7" t="s"/>
       <c r="H196" s="4" t="s"/>
-      <c r="I196" s="24" t="s"/>
-      <c r="J196" s="24" t="s"/>
-      <c r="K196" s="24" t="s"/>
+      <c r="I196" s="25" t="s"/>
+      <c r="J196" s="25" t="s"/>
+      <c r="K196" s="25" t="s"/>
       <c r="L196" s="7" t="s"/>
     </row>
     <row r="197" spans="1:12">
@@ -3971,9 +4056,9 @@
       <c r="F197" s="7" t="s"/>
       <c r="G197" s="7" t="s"/>
       <c r="H197" s="4" t="s"/>
-      <c r="I197" s="24" t="s"/>
-      <c r="J197" s="24" t="s"/>
-      <c r="K197" s="24" t="s"/>
+      <c r="I197" s="25" t="s"/>
+      <c r="J197" s="25" t="s"/>
+      <c r="K197" s="25" t="s"/>
       <c r="L197" s="7" t="s"/>
     </row>
     <row r="198" spans="1:12">
@@ -3985,9 +4070,9 @@
       <c r="F198" s="7" t="s"/>
       <c r="G198" s="7" t="s"/>
       <c r="H198" s="4" t="s"/>
-      <c r="I198" s="24" t="s"/>
-      <c r="J198" s="24" t="s"/>
-      <c r="K198" s="24" t="s"/>
+      <c r="I198" s="25" t="s"/>
+      <c r="J198" s="25" t="s"/>
+      <c r="K198" s="25" t="s"/>
       <c r="L198" s="7" t="s"/>
     </row>
     <row r="199" spans="1:12">
@@ -3999,9 +4084,9 @@
       <c r="F199" s="7" t="s"/>
       <c r="G199" s="7" t="s"/>
       <c r="H199" s="4" t="s"/>
-      <c r="I199" s="24" t="s"/>
-      <c r="J199" s="24" t="s"/>
-      <c r="K199" s="24" t="s"/>
+      <c r="I199" s="25" t="s"/>
+      <c r="J199" s="25" t="s"/>
+      <c r="K199" s="25" t="s"/>
       <c r="L199" s="7" t="s"/>
     </row>
     <row r="200" spans="1:12">
@@ -4013,9 +4098,9 @@
       <c r="F200" s="7" t="s"/>
       <c r="G200" s="7" t="s"/>
       <c r="H200" s="4" t="s"/>
-      <c r="I200" s="24" t="s"/>
-      <c r="J200" s="24" t="s"/>
-      <c r="K200" s="24" t="s"/>
+      <c r="I200" s="25" t="s"/>
+      <c r="J200" s="25" t="s"/>
+      <c r="K200" s="25" t="s"/>
       <c r="L200" s="7" t="s"/>
     </row>
     <row r="201" spans="1:12">
@@ -4027,9 +4112,9 @@
       <c r="F201" s="7" t="s"/>
       <c r="G201" s="7" t="s"/>
       <c r="H201" s="4" t="s"/>
-      <c r="I201" s="24" t="s"/>
-      <c r="J201" s="24" t="s"/>
-      <c r="K201" s="24" t="s"/>
+      <c r="I201" s="25" t="s"/>
+      <c r="J201" s="25" t="s"/>
+      <c r="K201" s="25" t="s"/>
       <c r="L201" s="7" t="s"/>
     </row>
     <row r="202" spans="1:12">
@@ -4041,9 +4126,9 @@
       <c r="F202" s="7" t="s"/>
       <c r="G202" s="7" t="s"/>
       <c r="H202" s="4" t="s"/>
-      <c r="I202" s="24" t="s"/>
-      <c r="J202" s="24" t="s"/>
-      <c r="K202" s="24" t="s"/>
+      <c r="I202" s="25" t="s"/>
+      <c r="J202" s="25" t="s"/>
+      <c r="K202" s="25" t="s"/>
       <c r="L202" s="7" t="s"/>
     </row>
     <row r="203" spans="1:12">
@@ -4055,9 +4140,9 @@
       <c r="F203" s="7" t="s"/>
       <c r="G203" s="7" t="s"/>
       <c r="H203" s="4" t="s"/>
-      <c r="I203" s="24" t="s"/>
-      <c r="J203" s="24" t="s"/>
-      <c r="K203" s="24" t="s"/>
+      <c r="I203" s="25" t="s"/>
+      <c r="J203" s="25" t="s"/>
+      <c r="K203" s="25" t="s"/>
       <c r="L203" s="7" t="s"/>
     </row>
     <row r="204" spans="1:12">
@@ -4069,9 +4154,9 @@
       <c r="F204" s="7" t="s"/>
       <c r="G204" s="7" t="s"/>
       <c r="H204" s="4" t="s"/>
-      <c r="I204" s="24" t="s"/>
-      <c r="J204" s="24" t="s"/>
-      <c r="K204" s="24" t="s"/>
+      <c r="I204" s="25" t="s"/>
+      <c r="J204" s="25" t="s"/>
+      <c r="K204" s="25" t="s"/>
       <c r="L204" s="7" t="s"/>
     </row>
     <row r="205" spans="1:12">
@@ -4083,9 +4168,9 @@
       <c r="F205" s="7" t="s"/>
       <c r="G205" s="7" t="s"/>
       <c r="H205" s="4" t="s"/>
-      <c r="I205" s="24" t="s"/>
-      <c r="J205" s="24" t="s"/>
-      <c r="K205" s="24" t="s"/>
+      <c r="I205" s="25" t="s"/>
+      <c r="J205" s="25" t="s"/>
+      <c r="K205" s="25" t="s"/>
       <c r="L205" s="7" t="s"/>
     </row>
     <row r="206" spans="1:12">
@@ -4097,9 +4182,9 @@
       <c r="F206" s="7" t="s"/>
       <c r="G206" s="7" t="s"/>
       <c r="H206" s="4" t="s"/>
-      <c r="I206" s="24" t="s"/>
-      <c r="J206" s="24" t="s"/>
-      <c r="K206" s="24" t="s"/>
+      <c r="I206" s="25" t="s"/>
+      <c r="J206" s="25" t="s"/>
+      <c r="K206" s="25" t="s"/>
       <c r="L206" s="7" t="s"/>
     </row>
     <row r="207" spans="1:12">
@@ -4111,11 +4196,29 @@
       <c r="F207" s="7" t="s"/>
       <c r="G207" s="7" t="s"/>
       <c r="H207" s="4" t="s"/>
-      <c r="I207" s="24" t="s"/>
-      <c r="J207" s="24" t="s"/>
-      <c r="K207" s="24" t="s"/>
+      <c r="I207" s="25" t="s"/>
+      <c r="J207" s="25" t="s"/>
+      <c r="K207" s="25" t="s"/>
       <c r="L207" s="7" t="s"/>
     </row>
+    <row r="208" spans="1:12">
+      <c r="A208" s="4" t="s"/>
+      <c r="B208" s="4" t="s"/>
+      <c r="C208" s="4" t="s"/>
+      <c r="D208" s="4" t="s"/>
+      <c r="E208" s="7" t="s"/>
+      <c r="F208" s="7" t="s"/>
+      <c r="G208" s="7" t="s"/>
+      <c r="H208" s="4" t="s"/>
+      <c r="I208" s="25" t="s"/>
+      <c r="J208" s="25" t="s"/>
+      <c r="K208" s="25" t="s"/>
+      <c r="L208" s="7" t="s"/>
+    </row>
   </sheetData>
+  <ignoredErrors>
+    <ignoredError sqref="E13" numberStoredAsText="true"/>
+    <ignoredError sqref="E21" numberStoredAsText="true"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>